<commit_message>
modif planification + ajout photos
</commit_message>
<xml_diff>
--- a/Documents/Planification_Projet_2026.xlsx
+++ b/Documents/Planification_Projet_2026.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\fauret.SNIRW\Projet_banc_test_self\Documents\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9340F35C-C567-4BF0-BAD6-0B2DF7FBC49F}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{474B44F3-0813-498B-8E5E-FBB7FB489C47}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12225" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -1456,7 +1456,7 @@
       <name val="Arial"/>
     </font>
   </fonts>
-  <fills count="9">
+  <fills count="10">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -1503,6 +1503,12 @@
       <patternFill patternType="solid">
         <fgColor rgb="FFFF8080"/>
         <bgColor rgb="FFFF8080"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
       </patternFill>
     </fill>
   </fills>
@@ -1935,7 +1941,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="92">
+  <cellXfs count="95">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -2088,6 +2094,13 @@
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="49" fontId="8" fillId="0" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="9" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="9" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="8" fillId="9" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -8163,8 +8176,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:AK1000"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A16" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="K40" sqref="K40"/>
+    <sheetView tabSelected="1" topLeftCell="A7" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="B10" sqref="B10:B11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="12.625" defaultRowHeight="15" customHeight="1"/>
@@ -8492,7 +8505,7 @@
         <v>#VALUE!</v>
       </c>
       <c r="H7" s="40"/>
-      <c r="I7" s="17"/>
+      <c r="I7" s="40"/>
       <c r="J7" s="17"/>
       <c r="K7" s="17"/>
       <c r="L7" s="18"/>
@@ -8614,7 +8627,7 @@
       <c r="A10" s="61" t="s">
         <v>53</v>
       </c>
-      <c r="B10" s="90" t="s">
+      <c r="B10" s="94" t="s">
         <v>67</v>
       </c>
       <c r="D10" s="22"/>
@@ -8657,7 +8670,7 @@
     </row>
     <row r="11" spans="1:37" ht="14.25" customHeight="1">
       <c r="A11" s="60"/>
-      <c r="B11" s="60"/>
+      <c r="B11" s="93"/>
       <c r="D11" s="54" t="s">
         <v>65</v>
       </c>
@@ -9416,7 +9429,7 @@
         <f t="array" aca="1" ref="G28" ca="1">IF(ISBLANK(INDIRECT(ADDRESS(ROW(),1,2,TRUE()))),"",IF((INDIRECT(ADDRESS(3,COLUMN(),2,1))="g"),"g"," "))</f>
         <v>#VALUE!</v>
       </c>
-      <c r="H28" s="17"/>
+      <c r="H28" s="35"/>
       <c r="I28" s="35"/>
       <c r="J28" s="17"/>
       <c r="K28" s="17"/>
@@ -9459,8 +9472,8 @@
         <f t="array" aca="1" ref="G29" ca="1">IF(ISBLANK(INDIRECT(ADDRESS(ROW()-1,1,2,TRUE()))),"",IF((INDIRECT(ADDRESS(3,COLUMN(),2,1))="g"),"g"," "))</f>
         <v>#VALUE!</v>
       </c>
-      <c r="H29" s="17"/>
-      <c r="I29" s="17"/>
+      <c r="H29" s="40"/>
+      <c r="I29" s="40"/>
       <c r="J29" s="17"/>
       <c r="K29" s="17"/>
       <c r="L29" s="18"/>
@@ -10198,7 +10211,7 @@
       <c r="A46" s="61" t="s">
         <v>91</v>
       </c>
-      <c r="B46" s="90" t="s">
+      <c r="B46" s="94" t="s">
         <v>67</v>
       </c>
       <c r="D46" s="22"/>
@@ -10241,7 +10254,7 @@
     </row>
     <row r="47" spans="1:37" ht="14.25" customHeight="1">
       <c r="A47" s="60"/>
-      <c r="B47" s="60"/>
+      <c r="B47" s="93"/>
       <c r="D47" s="19"/>
       <c r="E47" s="20"/>
       <c r="F47" s="55" t="s">
@@ -10286,7 +10299,7 @@
       <c r="A48" s="61" t="s">
         <v>92</v>
       </c>
-      <c r="B48" s="89" t="s">
+      <c r="B48" s="92" t="s">
         <v>93</v>
       </c>
       <c r="D48" s="22"/>
@@ -10329,7 +10342,7 @@
     </row>
     <row r="49" spans="1:37" ht="14.25" customHeight="1">
       <c r="A49" s="60"/>
-      <c r="B49" s="60"/>
+      <c r="B49" s="93"/>
       <c r="D49" s="19"/>
       <c r="E49" s="20"/>
       <c r="F49" s="55" t="s">

</xml_diff>

<commit_message>
Modification Journal + Plannification
</commit_message>
<xml_diff>
--- a/Documents/Planification_Projet_2026.xlsx
+++ b/Documents/Planification_Projet_2026.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\lerouxe.SNIRW\Projet_banc_test_self\Documents\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FD9E84B5-981B-4FF5-874F-E7AB33EBA531}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{55649459-8598-4EBA-B1E7-E6DEA77B3838}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12225" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView minimized="1" xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12225" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="SRC" sheetId="1" r:id="rId1"/>
@@ -2022,18 +2022,12 @@
       <alignment vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="10" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -2042,6 +2036,12 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="4" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
@@ -2065,13 +2065,13 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="29" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="30" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="31" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="10" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="10" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
@@ -2621,12 +2621,12 @@
       <c r="Y1" s="5" t="s">
         <v>1</v>
       </c>
-      <c r="Z1" s="59">
+      <c r="Z1" s="57">
         <v>2024</v>
       </c>
-      <c r="AA1" s="60"/>
-      <c r="AB1" s="60"/>
-      <c r="AC1" s="61"/>
+      <c r="AA1" s="58"/>
+      <c r="AB1" s="58"/>
+      <c r="AC1" s="59"/>
       <c r="AD1" s="6"/>
       <c r="AE1" s="4" t="s">
         <v>2</v>
@@ -2681,10 +2681,10 @@
       <c r="A3" s="11" t="s">
         <v>4</v>
       </c>
-      <c r="D3" s="62"/>
-      <c r="E3" s="63"/>
-      <c r="F3" s="63"/>
-      <c r="G3" s="63"/>
+      <c r="D3" s="60"/>
+      <c r="E3" s="61"/>
+      <c r="F3" s="61"/>
+      <c r="G3" s="61"/>
       <c r="I3" s="13" t="s">
         <v>5</v>
       </c>
@@ -2761,18 +2761,18 @@
       <c r="AL3" s="66"/>
     </row>
     <row r="4" spans="1:38" ht="14.25" customHeight="1">
-      <c r="D4" s="62"/>
-      <c r="E4" s="63"/>
-      <c r="F4" s="63"/>
-      <c r="G4" s="63"/>
+      <c r="D4" s="60"/>
+      <c r="E4" s="61"/>
+      <c r="F4" s="61"/>
+      <c r="G4" s="61"/>
       <c r="AD4" s="6"/>
       <c r="AE4" s="67"/>
-      <c r="AF4" s="63"/>
-      <c r="AG4" s="63"/>
-      <c r="AH4" s="63"/>
-      <c r="AI4" s="63"/>
-      <c r="AJ4" s="63"/>
-      <c r="AK4" s="63"/>
+      <c r="AF4" s="61"/>
+      <c r="AG4" s="61"/>
+      <c r="AH4" s="61"/>
+      <c r="AI4" s="61"/>
+      <c r="AJ4" s="61"/>
+      <c r="AK4" s="61"/>
       <c r="AL4" s="68"/>
     </row>
     <row r="5" spans="1:38" ht="14.25" customHeight="1">
@@ -2815,16 +2815,16 @@
       <c r="AC5" s="16"/>
       <c r="AD5" s="6"/>
       <c r="AE5" s="67"/>
-      <c r="AF5" s="63"/>
-      <c r="AG5" s="63"/>
-      <c r="AH5" s="63"/>
-      <c r="AI5" s="63"/>
-      <c r="AJ5" s="63"/>
-      <c r="AK5" s="63"/>
+      <c r="AF5" s="61"/>
+      <c r="AG5" s="61"/>
+      <c r="AH5" s="61"/>
+      <c r="AI5" s="61"/>
+      <c r="AJ5" s="61"/>
+      <c r="AK5" s="61"/>
       <c r="AL5" s="68"/>
     </row>
     <row r="6" spans="1:38" ht="15" customHeight="1">
-      <c r="A6" s="54" t="s">
+      <c r="A6" s="56" t="s">
         <v>30</v>
       </c>
       <c r="B6" s="72"/>
@@ -2856,12 +2856,12 @@
       <c r="AC6" s="17"/>
       <c r="AD6" s="6"/>
       <c r="AE6" s="67"/>
-      <c r="AF6" s="63"/>
-      <c r="AG6" s="63"/>
-      <c r="AH6" s="63"/>
-      <c r="AI6" s="63"/>
-      <c r="AJ6" s="63"/>
-      <c r="AK6" s="63"/>
+      <c r="AF6" s="61"/>
+      <c r="AG6" s="61"/>
+      <c r="AH6" s="61"/>
+      <c r="AI6" s="61"/>
+      <c r="AJ6" s="61"/>
+      <c r="AK6" s="61"/>
       <c r="AL6" s="68"/>
     </row>
     <row r="7" spans="1:38" ht="15" customHeight="1">
@@ -2895,19 +2895,19 @@
       <c r="AC7" s="17"/>
       <c r="AD7" s="6"/>
       <c r="AE7" s="67"/>
-      <c r="AF7" s="63"/>
-      <c r="AG7" s="63"/>
-      <c r="AH7" s="63"/>
-      <c r="AI7" s="63"/>
-      <c r="AJ7" s="63"/>
-      <c r="AK7" s="63"/>
+      <c r="AF7" s="61"/>
+      <c r="AG7" s="61"/>
+      <c r="AH7" s="61"/>
+      <c r="AI7" s="61"/>
+      <c r="AJ7" s="61"/>
+      <c r="AK7" s="61"/>
       <c r="AL7" s="68"/>
     </row>
     <row r="8" spans="1:38" ht="15" customHeight="1">
-      <c r="A8" s="54" t="s">
+      <c r="A8" s="56" t="s">
         <v>31</v>
       </c>
-      <c r="B8" s="56"/>
+      <c r="B8" s="63"/>
       <c r="D8" s="22"/>
       <c r="E8" s="22"/>
       <c r="F8" s="22"/>
@@ -2936,12 +2936,12 @@
       <c r="AC8" s="17"/>
       <c r="AD8" s="6"/>
       <c r="AE8" s="67"/>
-      <c r="AF8" s="63"/>
-      <c r="AG8" s="63"/>
-      <c r="AH8" s="63"/>
-      <c r="AI8" s="63"/>
-      <c r="AJ8" s="63"/>
-      <c r="AK8" s="63"/>
+      <c r="AF8" s="61"/>
+      <c r="AG8" s="61"/>
+      <c r="AH8" s="61"/>
+      <c r="AI8" s="61"/>
+      <c r="AJ8" s="61"/>
+      <c r="AK8" s="61"/>
       <c r="AL8" s="68"/>
     </row>
     <row r="9" spans="1:38" ht="15" customHeight="1">
@@ -2975,19 +2975,19 @@
       <c r="AC9" s="17"/>
       <c r="AD9" s="6"/>
       <c r="AE9" s="67"/>
-      <c r="AF9" s="63"/>
-      <c r="AG9" s="63"/>
-      <c r="AH9" s="63"/>
-      <c r="AI9" s="63"/>
-      <c r="AJ9" s="63"/>
-      <c r="AK9" s="63"/>
+      <c r="AF9" s="61"/>
+      <c r="AG9" s="61"/>
+      <c r="AH9" s="61"/>
+      <c r="AI9" s="61"/>
+      <c r="AJ9" s="61"/>
+      <c r="AK9" s="61"/>
       <c r="AL9" s="68"/>
     </row>
     <row r="10" spans="1:38" ht="15" customHeight="1">
-      <c r="A10" s="54" t="s">
+      <c r="A10" s="56" t="s">
         <v>32</v>
       </c>
-      <c r="B10" s="56"/>
+      <c r="B10" s="63"/>
       <c r="D10" s="22"/>
       <c r="E10" s="22"/>
       <c r="F10" s="22"/>
@@ -3016,12 +3016,12 @@
       <c r="AC10" s="17"/>
       <c r="AD10" s="6"/>
       <c r="AE10" s="67"/>
-      <c r="AF10" s="63"/>
-      <c r="AG10" s="63"/>
-      <c r="AH10" s="63"/>
-      <c r="AI10" s="63"/>
-      <c r="AJ10" s="63"/>
-      <c r="AK10" s="63"/>
+      <c r="AF10" s="61"/>
+      <c r="AG10" s="61"/>
+      <c r="AH10" s="61"/>
+      <c r="AI10" s="61"/>
+      <c r="AJ10" s="61"/>
+      <c r="AK10" s="61"/>
       <c r="AL10" s="68"/>
     </row>
     <row r="11" spans="1:38" ht="15" customHeight="1">
@@ -3055,19 +3055,19 @@
       <c r="AC11" s="17"/>
       <c r="AD11" s="6"/>
       <c r="AE11" s="67"/>
-      <c r="AF11" s="63"/>
-      <c r="AG11" s="63"/>
-      <c r="AH11" s="63"/>
-      <c r="AI11" s="63"/>
-      <c r="AJ11" s="63"/>
-      <c r="AK11" s="63"/>
+      <c r="AF11" s="61"/>
+      <c r="AG11" s="61"/>
+      <c r="AH11" s="61"/>
+      <c r="AI11" s="61"/>
+      <c r="AJ11" s="61"/>
+      <c r="AK11" s="61"/>
       <c r="AL11" s="68"/>
     </row>
     <row r="12" spans="1:38" ht="15" customHeight="1">
-      <c r="A12" s="54" t="s">
+      <c r="A12" s="56" t="s">
         <v>33</v>
       </c>
-      <c r="B12" s="56"/>
+      <c r="B12" s="63"/>
       <c r="D12" s="22"/>
       <c r="E12" s="22"/>
       <c r="F12" s="22"/>
@@ -3096,12 +3096,12 @@
       <c r="AC12" s="17"/>
       <c r="AD12" s="6"/>
       <c r="AE12" s="67"/>
-      <c r="AF12" s="63"/>
-      <c r="AG12" s="63"/>
-      <c r="AH12" s="63"/>
-      <c r="AI12" s="63"/>
-      <c r="AJ12" s="63"/>
-      <c r="AK12" s="63"/>
+      <c r="AF12" s="61"/>
+      <c r="AG12" s="61"/>
+      <c r="AH12" s="61"/>
+      <c r="AI12" s="61"/>
+      <c r="AJ12" s="61"/>
+      <c r="AK12" s="61"/>
       <c r="AL12" s="68"/>
     </row>
     <row r="13" spans="1:38" ht="15" customHeight="1">
@@ -3135,19 +3135,19 @@
       <c r="AC13" s="17"/>
       <c r="AD13" s="6"/>
       <c r="AE13" s="67"/>
-      <c r="AF13" s="63"/>
-      <c r="AG13" s="63"/>
-      <c r="AH13" s="63"/>
-      <c r="AI13" s="63"/>
-      <c r="AJ13" s="63"/>
-      <c r="AK13" s="63"/>
+      <c r="AF13" s="61"/>
+      <c r="AG13" s="61"/>
+      <c r="AH13" s="61"/>
+      <c r="AI13" s="61"/>
+      <c r="AJ13" s="61"/>
+      <c r="AK13" s="61"/>
       <c r="AL13" s="68"/>
     </row>
     <row r="14" spans="1:38" ht="15" customHeight="1">
-      <c r="A14" s="54" t="s">
+      <c r="A14" s="56" t="s">
         <v>34</v>
       </c>
-      <c r="B14" s="56"/>
+      <c r="B14" s="63"/>
       <c r="D14" s="22"/>
       <c r="E14" s="22"/>
       <c r="F14" s="22"/>
@@ -3176,12 +3176,12 @@
       <c r="AC14" s="17"/>
       <c r="AD14" s="6"/>
       <c r="AE14" s="67"/>
-      <c r="AF14" s="63"/>
-      <c r="AG14" s="63"/>
-      <c r="AH14" s="63"/>
-      <c r="AI14" s="63"/>
-      <c r="AJ14" s="63"/>
-      <c r="AK14" s="63"/>
+      <c r="AF14" s="61"/>
+      <c r="AG14" s="61"/>
+      <c r="AH14" s="61"/>
+      <c r="AI14" s="61"/>
+      <c r="AJ14" s="61"/>
+      <c r="AK14" s="61"/>
       <c r="AL14" s="68"/>
     </row>
     <row r="15" spans="1:38" ht="15" customHeight="1">
@@ -3215,19 +3215,19 @@
       <c r="AC15" s="17"/>
       <c r="AD15" s="6"/>
       <c r="AE15" s="67"/>
-      <c r="AF15" s="63"/>
-      <c r="AG15" s="63"/>
-      <c r="AH15" s="63"/>
-      <c r="AI15" s="63"/>
-      <c r="AJ15" s="63"/>
-      <c r="AK15" s="63"/>
+      <c r="AF15" s="61"/>
+      <c r="AG15" s="61"/>
+      <c r="AH15" s="61"/>
+      <c r="AI15" s="61"/>
+      <c r="AJ15" s="61"/>
+      <c r="AK15" s="61"/>
       <c r="AL15" s="68"/>
     </row>
     <row r="16" spans="1:38" ht="15" customHeight="1">
-      <c r="A16" s="54" t="s">
+      <c r="A16" s="56" t="s">
         <v>35</v>
       </c>
-      <c r="B16" s="57"/>
+      <c r="B16" s="54"/>
       <c r="D16" s="22"/>
       <c r="E16" s="22"/>
       <c r="F16" s="22"/>
@@ -3256,12 +3256,12 @@
       <c r="AC16" s="17"/>
       <c r="AD16" s="6"/>
       <c r="AE16" s="67"/>
-      <c r="AF16" s="63"/>
-      <c r="AG16" s="63"/>
-      <c r="AH16" s="63"/>
-      <c r="AI16" s="63"/>
-      <c r="AJ16" s="63"/>
-      <c r="AK16" s="63"/>
+      <c r="AF16" s="61"/>
+      <c r="AG16" s="61"/>
+      <c r="AH16" s="61"/>
+      <c r="AI16" s="61"/>
+      <c r="AJ16" s="61"/>
+      <c r="AK16" s="61"/>
       <c r="AL16" s="68"/>
     </row>
     <row r="17" spans="1:38" ht="15" customHeight="1">
@@ -3295,19 +3295,19 @@
       <c r="AC17" s="17"/>
       <c r="AD17" s="6"/>
       <c r="AE17" s="67"/>
-      <c r="AF17" s="63"/>
-      <c r="AG17" s="63"/>
-      <c r="AH17" s="63"/>
-      <c r="AI17" s="63"/>
-      <c r="AJ17" s="63"/>
-      <c r="AK17" s="63"/>
+      <c r="AF17" s="61"/>
+      <c r="AG17" s="61"/>
+      <c r="AH17" s="61"/>
+      <c r="AI17" s="61"/>
+      <c r="AJ17" s="61"/>
+      <c r="AK17" s="61"/>
       <c r="AL17" s="68"/>
     </row>
     <row r="18" spans="1:38" ht="15" customHeight="1">
-      <c r="A18" s="54" t="s">
+      <c r="A18" s="56" t="s">
         <v>36</v>
       </c>
-      <c r="B18" s="57"/>
+      <c r="B18" s="54"/>
       <c r="D18" s="22"/>
       <c r="E18" s="22"/>
       <c r="F18" s="22"/>
@@ -3336,12 +3336,12 @@
       <c r="AC18" s="17"/>
       <c r="AD18" s="6"/>
       <c r="AE18" s="67"/>
-      <c r="AF18" s="63"/>
-      <c r="AG18" s="63"/>
-      <c r="AH18" s="63"/>
-      <c r="AI18" s="63"/>
-      <c r="AJ18" s="63"/>
-      <c r="AK18" s="63"/>
+      <c r="AF18" s="61"/>
+      <c r="AG18" s="61"/>
+      <c r="AH18" s="61"/>
+      <c r="AI18" s="61"/>
+      <c r="AJ18" s="61"/>
+      <c r="AK18" s="61"/>
       <c r="AL18" s="68"/>
     </row>
     <row r="19" spans="1:38" ht="15" customHeight="1">
@@ -3375,19 +3375,19 @@
       <c r="AC19" s="17"/>
       <c r="AD19" s="6"/>
       <c r="AE19" s="67"/>
-      <c r="AF19" s="63"/>
-      <c r="AG19" s="63"/>
-      <c r="AH19" s="63"/>
-      <c r="AI19" s="63"/>
-      <c r="AJ19" s="63"/>
-      <c r="AK19" s="63"/>
+      <c r="AF19" s="61"/>
+      <c r="AG19" s="61"/>
+      <c r="AH19" s="61"/>
+      <c r="AI19" s="61"/>
+      <c r="AJ19" s="61"/>
+      <c r="AK19" s="61"/>
       <c r="AL19" s="68"/>
     </row>
     <row r="20" spans="1:38" ht="15" customHeight="1">
-      <c r="A20" s="54" t="s">
+      <c r="A20" s="56" t="s">
         <v>37</v>
       </c>
-      <c r="B20" s="57"/>
+      <c r="B20" s="54"/>
       <c r="D20" s="22"/>
       <c r="E20" s="22"/>
       <c r="F20" s="22"/>
@@ -3416,12 +3416,12 @@
       <c r="AC20" s="17"/>
       <c r="AD20" s="6"/>
       <c r="AE20" s="67"/>
-      <c r="AF20" s="63"/>
-      <c r="AG20" s="63"/>
-      <c r="AH20" s="63"/>
-      <c r="AI20" s="63"/>
-      <c r="AJ20" s="63"/>
-      <c r="AK20" s="63"/>
+      <c r="AF20" s="61"/>
+      <c r="AG20" s="61"/>
+      <c r="AH20" s="61"/>
+      <c r="AI20" s="61"/>
+      <c r="AJ20" s="61"/>
+      <c r="AK20" s="61"/>
       <c r="AL20" s="68"/>
     </row>
     <row r="21" spans="1:38" ht="15" customHeight="1">
@@ -3455,19 +3455,19 @@
       <c r="AC21" s="17"/>
       <c r="AD21" s="6"/>
       <c r="AE21" s="67"/>
-      <c r="AF21" s="63"/>
-      <c r="AG21" s="63"/>
-      <c r="AH21" s="63"/>
-      <c r="AI21" s="63"/>
-      <c r="AJ21" s="63"/>
-      <c r="AK21" s="63"/>
+      <c r="AF21" s="61"/>
+      <c r="AG21" s="61"/>
+      <c r="AH21" s="61"/>
+      <c r="AI21" s="61"/>
+      <c r="AJ21" s="61"/>
+      <c r="AK21" s="61"/>
       <c r="AL21" s="68"/>
     </row>
     <row r="22" spans="1:38" ht="15" customHeight="1">
-      <c r="A22" s="54" t="s">
+      <c r="A22" s="56" t="s">
         <v>38</v>
       </c>
-      <c r="B22" s="57"/>
+      <c r="B22" s="54"/>
       <c r="D22" s="22"/>
       <c r="E22" s="22"/>
       <c r="F22" s="22"/>
@@ -3496,12 +3496,12 @@
       <c r="AC22" s="17"/>
       <c r="AD22" s="6"/>
       <c r="AE22" s="67"/>
-      <c r="AF22" s="63"/>
-      <c r="AG22" s="63"/>
-      <c r="AH22" s="63"/>
-      <c r="AI22" s="63"/>
-      <c r="AJ22" s="63"/>
-      <c r="AK22" s="63"/>
+      <c r="AF22" s="61"/>
+      <c r="AG22" s="61"/>
+      <c r="AH22" s="61"/>
+      <c r="AI22" s="61"/>
+      <c r="AJ22" s="61"/>
+      <c r="AK22" s="61"/>
       <c r="AL22" s="68"/>
     </row>
     <row r="23" spans="1:38" ht="15" customHeight="1">
@@ -3535,19 +3535,19 @@
       <c r="AC23" s="17"/>
       <c r="AD23" s="6"/>
       <c r="AE23" s="67"/>
-      <c r="AF23" s="63"/>
-      <c r="AG23" s="63"/>
-      <c r="AH23" s="63"/>
-      <c r="AI23" s="63"/>
-      <c r="AJ23" s="63"/>
-      <c r="AK23" s="63"/>
+      <c r="AF23" s="61"/>
+      <c r="AG23" s="61"/>
+      <c r="AH23" s="61"/>
+      <c r="AI23" s="61"/>
+      <c r="AJ23" s="61"/>
+      <c r="AK23" s="61"/>
       <c r="AL23" s="68"/>
     </row>
     <row r="24" spans="1:38" ht="15" customHeight="1">
-      <c r="A24" s="54" t="s">
+      <c r="A24" s="56" t="s">
         <v>39</v>
       </c>
-      <c r="B24" s="57"/>
+      <c r="B24" s="54"/>
       <c r="D24" s="22"/>
       <c r="E24" s="22"/>
       <c r="F24" s="22"/>
@@ -3576,12 +3576,12 @@
       <c r="AC24" s="17"/>
       <c r="AD24" s="6"/>
       <c r="AE24" s="67"/>
-      <c r="AF24" s="63"/>
-      <c r="AG24" s="63"/>
-      <c r="AH24" s="63"/>
-      <c r="AI24" s="63"/>
-      <c r="AJ24" s="63"/>
-      <c r="AK24" s="63"/>
+      <c r="AF24" s="61"/>
+      <c r="AG24" s="61"/>
+      <c r="AH24" s="61"/>
+      <c r="AI24" s="61"/>
+      <c r="AJ24" s="61"/>
+      <c r="AK24" s="61"/>
       <c r="AL24" s="68"/>
     </row>
     <row r="25" spans="1:38" ht="15" customHeight="1">
@@ -3615,19 +3615,19 @@
       <c r="AC25" s="17"/>
       <c r="AD25" s="6"/>
       <c r="AE25" s="67"/>
-      <c r="AF25" s="63"/>
-      <c r="AG25" s="63"/>
-      <c r="AH25" s="63"/>
-      <c r="AI25" s="63"/>
-      <c r="AJ25" s="63"/>
-      <c r="AK25" s="63"/>
+      <c r="AF25" s="61"/>
+      <c r="AG25" s="61"/>
+      <c r="AH25" s="61"/>
+      <c r="AI25" s="61"/>
+      <c r="AJ25" s="61"/>
+      <c r="AK25" s="61"/>
       <c r="AL25" s="68"/>
     </row>
     <row r="26" spans="1:38" ht="15" customHeight="1">
-      <c r="A26" s="54" t="s">
+      <c r="A26" s="56" t="s">
         <v>40</v>
       </c>
-      <c r="B26" s="57"/>
+      <c r="B26" s="54"/>
       <c r="D26" s="22"/>
       <c r="E26" s="22"/>
       <c r="F26" s="22"/>
@@ -3656,12 +3656,12 @@
       <c r="AC26" s="17"/>
       <c r="AD26" s="6"/>
       <c r="AE26" s="67"/>
-      <c r="AF26" s="63"/>
-      <c r="AG26" s="63"/>
-      <c r="AH26" s="63"/>
-      <c r="AI26" s="63"/>
-      <c r="AJ26" s="63"/>
-      <c r="AK26" s="63"/>
+      <c r="AF26" s="61"/>
+      <c r="AG26" s="61"/>
+      <c r="AH26" s="61"/>
+      <c r="AI26" s="61"/>
+      <c r="AJ26" s="61"/>
+      <c r="AK26" s="61"/>
       <c r="AL26" s="68"/>
     </row>
     <row r="27" spans="1:38" ht="15" customHeight="1">
@@ -3695,19 +3695,19 @@
       <c r="AC27" s="17"/>
       <c r="AD27" s="6"/>
       <c r="AE27" s="67"/>
-      <c r="AF27" s="63"/>
-      <c r="AG27" s="63"/>
-      <c r="AH27" s="63"/>
-      <c r="AI27" s="63"/>
-      <c r="AJ27" s="63"/>
-      <c r="AK27" s="63"/>
+      <c r="AF27" s="61"/>
+      <c r="AG27" s="61"/>
+      <c r="AH27" s="61"/>
+      <c r="AI27" s="61"/>
+      <c r="AJ27" s="61"/>
+      <c r="AK27" s="61"/>
       <c r="AL27" s="68"/>
     </row>
     <row r="28" spans="1:38" ht="15" customHeight="1">
-      <c r="A28" s="54" t="s">
+      <c r="A28" s="56" t="s">
         <v>41</v>
       </c>
-      <c r="B28" s="57"/>
+      <c r="B28" s="54"/>
       <c r="D28" s="22"/>
       <c r="E28" s="22"/>
       <c r="F28" s="22"/>
@@ -3736,12 +3736,12 @@
       <c r="AC28" s="17"/>
       <c r="AD28" s="6"/>
       <c r="AE28" s="67"/>
-      <c r="AF28" s="63"/>
-      <c r="AG28" s="63"/>
-      <c r="AH28" s="63"/>
-      <c r="AI28" s="63"/>
-      <c r="AJ28" s="63"/>
-      <c r="AK28" s="63"/>
+      <c r="AF28" s="61"/>
+      <c r="AG28" s="61"/>
+      <c r="AH28" s="61"/>
+      <c r="AI28" s="61"/>
+      <c r="AJ28" s="61"/>
+      <c r="AK28" s="61"/>
       <c r="AL28" s="68"/>
     </row>
     <row r="29" spans="1:38" ht="15" customHeight="1">
@@ -3775,19 +3775,19 @@
       <c r="AC29" s="17"/>
       <c r="AD29" s="6"/>
       <c r="AE29" s="67"/>
-      <c r="AF29" s="63"/>
-      <c r="AG29" s="63"/>
-      <c r="AH29" s="63"/>
-      <c r="AI29" s="63"/>
-      <c r="AJ29" s="63"/>
-      <c r="AK29" s="63"/>
+      <c r="AF29" s="61"/>
+      <c r="AG29" s="61"/>
+      <c r="AH29" s="61"/>
+      <c r="AI29" s="61"/>
+      <c r="AJ29" s="61"/>
+      <c r="AK29" s="61"/>
       <c r="AL29" s="68"/>
     </row>
     <row r="30" spans="1:38" ht="15" customHeight="1">
-      <c r="A30" s="54" t="s">
+      <c r="A30" s="56" t="s">
         <v>42</v>
       </c>
-      <c r="B30" s="57"/>
+      <c r="B30" s="54"/>
       <c r="D30" s="22"/>
       <c r="E30" s="22"/>
       <c r="F30" s="22"/>
@@ -3816,12 +3816,12 @@
       <c r="AC30" s="17"/>
       <c r="AD30" s="6"/>
       <c r="AE30" s="67"/>
-      <c r="AF30" s="63"/>
-      <c r="AG30" s="63"/>
-      <c r="AH30" s="63"/>
-      <c r="AI30" s="63"/>
-      <c r="AJ30" s="63"/>
-      <c r="AK30" s="63"/>
+      <c r="AF30" s="61"/>
+      <c r="AG30" s="61"/>
+      <c r="AH30" s="61"/>
+      <c r="AI30" s="61"/>
+      <c r="AJ30" s="61"/>
+      <c r="AK30" s="61"/>
       <c r="AL30" s="68"/>
     </row>
     <row r="31" spans="1:38" ht="15" customHeight="1">
@@ -3855,19 +3855,19 @@
       <c r="AC31" s="17"/>
       <c r="AD31" s="6"/>
       <c r="AE31" s="67"/>
-      <c r="AF31" s="63"/>
-      <c r="AG31" s="63"/>
-      <c r="AH31" s="63"/>
-      <c r="AI31" s="63"/>
-      <c r="AJ31" s="63"/>
-      <c r="AK31" s="63"/>
+      <c r="AF31" s="61"/>
+      <c r="AG31" s="61"/>
+      <c r="AH31" s="61"/>
+      <c r="AI31" s="61"/>
+      <c r="AJ31" s="61"/>
+      <c r="AK31" s="61"/>
       <c r="AL31" s="68"/>
     </row>
     <row r="32" spans="1:38" ht="15" customHeight="1">
-      <c r="A32" s="54" t="s">
+      <c r="A32" s="56" t="s">
         <v>43</v>
       </c>
-      <c r="B32" s="82"/>
+      <c r="B32" s="81"/>
       <c r="D32" s="22"/>
       <c r="E32" s="22"/>
       <c r="F32" s="22"/>
@@ -3896,12 +3896,12 @@
       <c r="AC32" s="17"/>
       <c r="AD32" s="6"/>
       <c r="AE32" s="67"/>
-      <c r="AF32" s="63"/>
-      <c r="AG32" s="63"/>
-      <c r="AH32" s="63"/>
-      <c r="AI32" s="63"/>
-      <c r="AJ32" s="63"/>
-      <c r="AK32" s="63"/>
+      <c r="AF32" s="61"/>
+      <c r="AG32" s="61"/>
+      <c r="AH32" s="61"/>
+      <c r="AI32" s="61"/>
+      <c r="AJ32" s="61"/>
+      <c r="AK32" s="61"/>
       <c r="AL32" s="68"/>
     </row>
     <row r="33" spans="1:38" ht="15" customHeight="1">
@@ -3935,19 +3935,19 @@
       <c r="AC33" s="17"/>
       <c r="AD33" s="6"/>
       <c r="AE33" s="67"/>
-      <c r="AF33" s="63"/>
-      <c r="AG33" s="63"/>
-      <c r="AH33" s="63"/>
-      <c r="AI33" s="63"/>
-      <c r="AJ33" s="63"/>
-      <c r="AK33" s="63"/>
+      <c r="AF33" s="61"/>
+      <c r="AG33" s="61"/>
+      <c r="AH33" s="61"/>
+      <c r="AI33" s="61"/>
+      <c r="AJ33" s="61"/>
+      <c r="AK33" s="61"/>
       <c r="AL33" s="68"/>
     </row>
     <row r="34" spans="1:38" ht="15" customHeight="1">
-      <c r="A34" s="54" t="s">
+      <c r="A34" s="56" t="s">
         <v>44</v>
       </c>
-      <c r="B34" s="83"/>
+      <c r="B34" s="82"/>
       <c r="D34" s="22"/>
       <c r="E34" s="22"/>
       <c r="F34" s="22"/>
@@ -3976,12 +3976,12 @@
       <c r="AC34" s="17"/>
       <c r="AD34" s="6"/>
       <c r="AE34" s="67"/>
-      <c r="AF34" s="63"/>
-      <c r="AG34" s="63"/>
-      <c r="AH34" s="63"/>
-      <c r="AI34" s="63"/>
-      <c r="AJ34" s="63"/>
-      <c r="AK34" s="63"/>
+      <c r="AF34" s="61"/>
+      <c r="AG34" s="61"/>
+      <c r="AH34" s="61"/>
+      <c r="AI34" s="61"/>
+      <c r="AJ34" s="61"/>
+      <c r="AK34" s="61"/>
       <c r="AL34" s="68"/>
     </row>
     <row r="35" spans="1:38" ht="15" customHeight="1">
@@ -4024,10 +4024,10 @@
       <c r="AL35" s="71"/>
     </row>
     <row r="36" spans="1:38" ht="15" customHeight="1">
-      <c r="A36" s="54" t="s">
+      <c r="A36" s="56" t="s">
         <v>45</v>
       </c>
-      <c r="B36" s="57"/>
+      <c r="B36" s="54"/>
       <c r="D36" s="22"/>
       <c r="E36" s="22"/>
       <c r="F36" s="22"/>
@@ -4104,10 +4104,10 @@
       <c r="AL37" s="6"/>
     </row>
     <row r="38" spans="1:38" ht="15" customHeight="1">
-      <c r="A38" s="54" t="s">
+      <c r="A38" s="56" t="s">
         <v>46</v>
       </c>
-      <c r="B38" s="57"/>
+      <c r="B38" s="54"/>
       <c r="D38" s="22"/>
       <c r="E38" s="22"/>
       <c r="F38" s="22"/>
@@ -4186,10 +4186,10 @@
       <c r="AL39" s="75"/>
     </row>
     <row r="40" spans="1:38" ht="15" customHeight="1">
-      <c r="A40" s="54" t="s">
+      <c r="A40" s="56" t="s">
         <v>48</v>
       </c>
-      <c r="B40" s="57"/>
+      <c r="B40" s="54"/>
       <c r="D40" s="22"/>
       <c r="E40" s="22"/>
       <c r="F40" s="22"/>
@@ -4218,12 +4218,12 @@
       <c r="AC40" s="17"/>
       <c r="AD40" s="6"/>
       <c r="AE40" s="76"/>
-      <c r="AF40" s="63"/>
-      <c r="AG40" s="63"/>
-      <c r="AH40" s="63"/>
-      <c r="AI40" s="63"/>
-      <c r="AJ40" s="63"/>
-      <c r="AK40" s="63"/>
+      <c r="AF40" s="61"/>
+      <c r="AG40" s="61"/>
+      <c r="AH40" s="61"/>
+      <c r="AI40" s="61"/>
+      <c r="AJ40" s="61"/>
+      <c r="AK40" s="61"/>
       <c r="AL40" s="77"/>
     </row>
     <row r="41" spans="1:38" ht="15" customHeight="1">
@@ -4257,19 +4257,19 @@
       <c r="AC41" s="17"/>
       <c r="AD41" s="6"/>
       <c r="AE41" s="76"/>
-      <c r="AF41" s="63"/>
-      <c r="AG41" s="63"/>
-      <c r="AH41" s="63"/>
-      <c r="AI41" s="63"/>
-      <c r="AJ41" s="63"/>
-      <c r="AK41" s="63"/>
+      <c r="AF41" s="61"/>
+      <c r="AG41" s="61"/>
+      <c r="AH41" s="61"/>
+      <c r="AI41" s="61"/>
+      <c r="AJ41" s="61"/>
+      <c r="AK41" s="61"/>
       <c r="AL41" s="77"/>
     </row>
     <row r="42" spans="1:38" ht="15" customHeight="1">
-      <c r="A42" s="54" t="s">
+      <c r="A42" s="56" t="s">
         <v>49</v>
       </c>
-      <c r="B42" s="57"/>
+      <c r="B42" s="54"/>
       <c r="D42" s="22"/>
       <c r="E42" s="22"/>
       <c r="F42" s="22"/>
@@ -4298,12 +4298,12 @@
       <c r="AC42" s="17"/>
       <c r="AD42" s="6"/>
       <c r="AE42" s="76"/>
-      <c r="AF42" s="63"/>
-      <c r="AG42" s="63"/>
-      <c r="AH42" s="63"/>
-      <c r="AI42" s="63"/>
-      <c r="AJ42" s="63"/>
-      <c r="AK42" s="63"/>
+      <c r="AF42" s="61"/>
+      <c r="AG42" s="61"/>
+      <c r="AH42" s="61"/>
+      <c r="AI42" s="61"/>
+      <c r="AJ42" s="61"/>
+      <c r="AK42" s="61"/>
       <c r="AL42" s="77"/>
     </row>
     <row r="43" spans="1:38" ht="15" customHeight="1">
@@ -4337,19 +4337,19 @@
       <c r="AC43" s="17"/>
       <c r="AD43" s="6"/>
       <c r="AE43" s="76"/>
-      <c r="AF43" s="63"/>
-      <c r="AG43" s="63"/>
-      <c r="AH43" s="63"/>
-      <c r="AI43" s="63"/>
-      <c r="AJ43" s="63"/>
-      <c r="AK43" s="63"/>
+      <c r="AF43" s="61"/>
+      <c r="AG43" s="61"/>
+      <c r="AH43" s="61"/>
+      <c r="AI43" s="61"/>
+      <c r="AJ43" s="61"/>
+      <c r="AK43" s="61"/>
       <c r="AL43" s="77"/>
     </row>
     <row r="44" spans="1:38" ht="15" customHeight="1">
-      <c r="A44" s="54" t="s">
+      <c r="A44" s="56" t="s">
         <v>50</v>
       </c>
-      <c r="B44" s="58"/>
+      <c r="B44" s="62"/>
       <c r="D44" s="22"/>
       <c r="E44" s="22"/>
       <c r="F44" s="22"/>
@@ -4378,12 +4378,12 @@
       <c r="AC44" s="17"/>
       <c r="AD44" s="6"/>
       <c r="AE44" s="76"/>
-      <c r="AF44" s="63"/>
-      <c r="AG44" s="63"/>
-      <c r="AH44" s="63"/>
-      <c r="AI44" s="63"/>
-      <c r="AJ44" s="63"/>
-      <c r="AK44" s="63"/>
+      <c r="AF44" s="61"/>
+      <c r="AG44" s="61"/>
+      <c r="AH44" s="61"/>
+      <c r="AI44" s="61"/>
+      <c r="AJ44" s="61"/>
+      <c r="AK44" s="61"/>
       <c r="AL44" s="77"/>
     </row>
     <row r="45" spans="1:38" ht="15" customHeight="1">
@@ -4417,19 +4417,19 @@
       <c r="AC45" s="17"/>
       <c r="AD45" s="6"/>
       <c r="AE45" s="76"/>
-      <c r="AF45" s="63"/>
-      <c r="AG45" s="63"/>
-      <c r="AH45" s="63"/>
-      <c r="AI45" s="63"/>
-      <c r="AJ45" s="63"/>
-      <c r="AK45" s="63"/>
+      <c r="AF45" s="61"/>
+      <c r="AG45" s="61"/>
+      <c r="AH45" s="61"/>
+      <c r="AI45" s="61"/>
+      <c r="AJ45" s="61"/>
+      <c r="AK45" s="61"/>
       <c r="AL45" s="77"/>
     </row>
     <row r="46" spans="1:38" ht="15" customHeight="1">
-      <c r="A46" s="54" t="s">
+      <c r="A46" s="56" t="s">
         <v>51</v>
       </c>
-      <c r="B46" s="57"/>
+      <c r="B46" s="54"/>
       <c r="D46" s="22"/>
       <c r="E46" s="22"/>
       <c r="F46" s="22"/>
@@ -4458,12 +4458,12 @@
       <c r="AC46" s="17"/>
       <c r="AD46" s="6"/>
       <c r="AE46" s="76"/>
-      <c r="AF46" s="63"/>
-      <c r="AG46" s="63"/>
-      <c r="AH46" s="63"/>
-      <c r="AI46" s="63"/>
-      <c r="AJ46" s="63"/>
-      <c r="AK46" s="63"/>
+      <c r="AF46" s="61"/>
+      <c r="AG46" s="61"/>
+      <c r="AH46" s="61"/>
+      <c r="AI46" s="61"/>
+      <c r="AJ46" s="61"/>
+      <c r="AK46" s="61"/>
       <c r="AL46" s="77"/>
     </row>
     <row r="47" spans="1:38" ht="15" customHeight="1">
@@ -4497,19 +4497,19 @@
       <c r="AC47" s="17"/>
       <c r="AD47" s="6"/>
       <c r="AE47" s="76"/>
-      <c r="AF47" s="63"/>
-      <c r="AG47" s="63"/>
-      <c r="AH47" s="63"/>
-      <c r="AI47" s="63"/>
-      <c r="AJ47" s="63"/>
-      <c r="AK47" s="63"/>
+      <c r="AF47" s="61"/>
+      <c r="AG47" s="61"/>
+      <c r="AH47" s="61"/>
+      <c r="AI47" s="61"/>
+      <c r="AJ47" s="61"/>
+      <c r="AK47" s="61"/>
       <c r="AL47" s="77"/>
     </row>
     <row r="48" spans="1:38" ht="15" customHeight="1">
-      <c r="A48" s="54" t="s">
+      <c r="A48" s="56" t="s">
         <v>52</v>
       </c>
-      <c r="B48" s="57"/>
+      <c r="B48" s="54"/>
       <c r="D48" s="22"/>
       <c r="E48" s="22"/>
       <c r="F48" s="22"/>
@@ -4538,12 +4538,12 @@
       <c r="AC48" s="17"/>
       <c r="AD48" s="6"/>
       <c r="AE48" s="76"/>
-      <c r="AF48" s="63"/>
-      <c r="AG48" s="63"/>
-      <c r="AH48" s="63"/>
-      <c r="AI48" s="63"/>
-      <c r="AJ48" s="63"/>
-      <c r="AK48" s="63"/>
+      <c r="AF48" s="61"/>
+      <c r="AG48" s="61"/>
+      <c r="AH48" s="61"/>
+      <c r="AI48" s="61"/>
+      <c r="AJ48" s="61"/>
+      <c r="AK48" s="61"/>
       <c r="AL48" s="77"/>
     </row>
     <row r="49" spans="1:38" ht="15" customHeight="1">
@@ -4577,19 +4577,19 @@
       <c r="AC49" s="17"/>
       <c r="AD49" s="6"/>
       <c r="AE49" s="76"/>
-      <c r="AF49" s="63"/>
-      <c r="AG49" s="63"/>
-      <c r="AH49" s="63"/>
-      <c r="AI49" s="63"/>
-      <c r="AJ49" s="63"/>
-      <c r="AK49" s="63"/>
+      <c r="AF49" s="61"/>
+      <c r="AG49" s="61"/>
+      <c r="AH49" s="61"/>
+      <c r="AI49" s="61"/>
+      <c r="AJ49" s="61"/>
+      <c r="AK49" s="61"/>
       <c r="AL49" s="77"/>
     </row>
     <row r="50" spans="1:38" ht="15" customHeight="1">
-      <c r="A50" s="54" t="s">
+      <c r="A50" s="56" t="s">
         <v>53</v>
       </c>
-      <c r="B50" s="57"/>
+      <c r="B50" s="54"/>
       <c r="D50" s="22"/>
       <c r="E50" s="22"/>
       <c r="F50" s="22"/>
@@ -4618,12 +4618,12 @@
       <c r="AC50" s="17"/>
       <c r="AD50" s="6"/>
       <c r="AE50" s="76"/>
-      <c r="AF50" s="63"/>
-      <c r="AG50" s="63"/>
-      <c r="AH50" s="63"/>
-      <c r="AI50" s="63"/>
-      <c r="AJ50" s="63"/>
-      <c r="AK50" s="63"/>
+      <c r="AF50" s="61"/>
+      <c r="AG50" s="61"/>
+      <c r="AH50" s="61"/>
+      <c r="AI50" s="61"/>
+      <c r="AJ50" s="61"/>
+      <c r="AK50" s="61"/>
       <c r="AL50" s="77"/>
     </row>
     <row r="51" spans="1:38" ht="15" customHeight="1">
@@ -4657,19 +4657,19 @@
       <c r="AC51" s="17"/>
       <c r="AD51" s="6"/>
       <c r="AE51" s="76"/>
-      <c r="AF51" s="63"/>
-      <c r="AG51" s="63"/>
-      <c r="AH51" s="63"/>
-      <c r="AI51" s="63"/>
-      <c r="AJ51" s="63"/>
-      <c r="AK51" s="63"/>
+      <c r="AF51" s="61"/>
+      <c r="AG51" s="61"/>
+      <c r="AH51" s="61"/>
+      <c r="AI51" s="61"/>
+      <c r="AJ51" s="61"/>
+      <c r="AK51" s="61"/>
       <c r="AL51" s="77"/>
     </row>
     <row r="52" spans="1:38" ht="15" customHeight="1">
-      <c r="A52" s="54" t="s">
+      <c r="A52" s="56" t="s">
         <v>54</v>
       </c>
-      <c r="B52" s="57"/>
+      <c r="B52" s="54"/>
       <c r="D52" s="22"/>
       <c r="E52" s="22"/>
       <c r="F52" s="22"/>
@@ -4698,12 +4698,12 @@
       <c r="AC52" s="17"/>
       <c r="AD52" s="6"/>
       <c r="AE52" s="76"/>
-      <c r="AF52" s="63"/>
-      <c r="AG52" s="63"/>
-      <c r="AH52" s="63"/>
-      <c r="AI52" s="63"/>
-      <c r="AJ52" s="63"/>
-      <c r="AK52" s="63"/>
+      <c r="AF52" s="61"/>
+      <c r="AG52" s="61"/>
+      <c r="AH52" s="61"/>
+      <c r="AI52" s="61"/>
+      <c r="AJ52" s="61"/>
+      <c r="AK52" s="61"/>
       <c r="AL52" s="77"/>
     </row>
     <row r="53" spans="1:38" ht="15" customHeight="1">
@@ -4737,19 +4737,19 @@
       <c r="AC53" s="17"/>
       <c r="AD53" s="6"/>
       <c r="AE53" s="76"/>
-      <c r="AF53" s="63"/>
-      <c r="AG53" s="63"/>
-      <c r="AH53" s="63"/>
-      <c r="AI53" s="63"/>
-      <c r="AJ53" s="63"/>
-      <c r="AK53" s="63"/>
+      <c r="AF53" s="61"/>
+      <c r="AG53" s="61"/>
+      <c r="AH53" s="61"/>
+      <c r="AI53" s="61"/>
+      <c r="AJ53" s="61"/>
+      <c r="AK53" s="61"/>
       <c r="AL53" s="77"/>
     </row>
     <row r="54" spans="1:38" ht="15" customHeight="1">
-      <c r="A54" s="54" t="s">
+      <c r="A54" s="56" t="s">
         <v>55</v>
       </c>
-      <c r="B54" s="57"/>
+      <c r="B54" s="54"/>
       <c r="D54" s="22"/>
       <c r="E54" s="22"/>
       <c r="F54" s="22"/>
@@ -4778,12 +4778,12 @@
       <c r="AC54" s="17"/>
       <c r="AD54" s="6"/>
       <c r="AE54" s="76"/>
-      <c r="AF54" s="63"/>
-      <c r="AG54" s="63"/>
-      <c r="AH54" s="63"/>
-      <c r="AI54" s="63"/>
-      <c r="AJ54" s="63"/>
-      <c r="AK54" s="63"/>
+      <c r="AF54" s="61"/>
+      <c r="AG54" s="61"/>
+      <c r="AH54" s="61"/>
+      <c r="AI54" s="61"/>
+      <c r="AJ54" s="61"/>
+      <c r="AK54" s="61"/>
       <c r="AL54" s="77"/>
     </row>
     <row r="55" spans="1:38" ht="15" customHeight="1">
@@ -4817,19 +4817,19 @@
       <c r="AC55" s="17"/>
       <c r="AD55" s="6"/>
       <c r="AE55" s="76"/>
-      <c r="AF55" s="63"/>
-      <c r="AG55" s="63"/>
-      <c r="AH55" s="63"/>
-      <c r="AI55" s="63"/>
-      <c r="AJ55" s="63"/>
-      <c r="AK55" s="63"/>
+      <c r="AF55" s="61"/>
+      <c r="AG55" s="61"/>
+      <c r="AH55" s="61"/>
+      <c r="AI55" s="61"/>
+      <c r="AJ55" s="61"/>
+      <c r="AK55" s="61"/>
       <c r="AL55" s="77"/>
     </row>
     <row r="56" spans="1:38" ht="15" customHeight="1">
-      <c r="A56" s="54" t="s">
+      <c r="A56" s="56" t="s">
         <v>56</v>
       </c>
-      <c r="B56" s="57"/>
+      <c r="B56" s="54"/>
       <c r="D56" s="22"/>
       <c r="E56" s="22"/>
       <c r="F56" s="22"/>
@@ -4908,10 +4908,10 @@
       <c r="AL57" s="38"/>
     </row>
     <row r="58" spans="1:38" ht="15" customHeight="1">
-      <c r="A58" s="54" t="s">
+      <c r="A58" s="56" t="s">
         <v>58</v>
       </c>
-      <c r="B58" s="57"/>
+      <c r="B58" s="54"/>
       <c r="D58" s="22"/>
       <c r="E58" s="22"/>
       <c r="F58" s="22"/>
@@ -4992,8 +4992,8 @@
       <c r="AL59" s="38"/>
     </row>
     <row r="60" spans="1:38" ht="15" customHeight="1">
-      <c r="A60" s="81"/>
-      <c r="B60" s="81"/>
+      <c r="A60" s="83"/>
+      <c r="B60" s="83"/>
       <c r="D60" s="22"/>
       <c r="E60" s="22"/>
       <c r="F60" s="22"/>
@@ -5074,8 +5074,8 @@
       <c r="AL61" s="38"/>
     </row>
     <row r="62" spans="1:38" ht="15" customHeight="1">
-      <c r="A62" s="81"/>
-      <c r="B62" s="81"/>
+      <c r="A62" s="83"/>
+      <c r="B62" s="83"/>
       <c r="D62" s="22"/>
       <c r="E62" s="22"/>
       <c r="F62" s="22"/>
@@ -5154,8 +5154,8 @@
       <c r="AL63" s="38"/>
     </row>
     <row r="64" spans="1:38" ht="15" customHeight="1">
-      <c r="A64" s="81"/>
-      <c r="B64" s="81"/>
+      <c r="A64" s="83"/>
+      <c r="B64" s="83"/>
       <c r="D64" s="22"/>
       <c r="E64" s="22"/>
       <c r="F64" s="22"/>
@@ -8074,13 +8074,20 @@
     </row>
   </sheetData>
   <mergeCells count="65">
-    <mergeCell ref="A48:A49"/>
     <mergeCell ref="A50:A51"/>
     <mergeCell ref="A6:A7"/>
     <mergeCell ref="A40:A41"/>
     <mergeCell ref="A42:A43"/>
     <mergeCell ref="A44:A45"/>
     <mergeCell ref="A46:A47"/>
+    <mergeCell ref="A18:A19"/>
+    <mergeCell ref="A20:A21"/>
+    <mergeCell ref="A22:A23"/>
+    <mergeCell ref="A8:A9"/>
+    <mergeCell ref="A10:A11"/>
+    <mergeCell ref="A14:A15"/>
+    <mergeCell ref="A16:A17"/>
+    <mergeCell ref="A12:A13"/>
     <mergeCell ref="A52:A53"/>
     <mergeCell ref="A54:A55"/>
     <mergeCell ref="A56:A57"/>
@@ -8108,12 +8115,17 @@
     <mergeCell ref="B50:B51"/>
     <mergeCell ref="B52:B53"/>
     <mergeCell ref="B54:B55"/>
+    <mergeCell ref="B46:B47"/>
     <mergeCell ref="Z1:AC1"/>
     <mergeCell ref="D3:G3"/>
     <mergeCell ref="B40:B41"/>
     <mergeCell ref="B42:B43"/>
     <mergeCell ref="B44:B45"/>
-    <mergeCell ref="B46:B47"/>
+    <mergeCell ref="B18:B19"/>
+    <mergeCell ref="B20:B21"/>
+    <mergeCell ref="B22:B23"/>
+    <mergeCell ref="B14:B15"/>
+    <mergeCell ref="B16:B17"/>
     <mergeCell ref="B48:B49"/>
     <mergeCell ref="A24:A25"/>
     <mergeCell ref="B24:B25"/>
@@ -8126,19 +8138,7 @@
     <mergeCell ref="A30:A31"/>
     <mergeCell ref="A32:A33"/>
     <mergeCell ref="A34:A35"/>
-    <mergeCell ref="A18:A19"/>
-    <mergeCell ref="B18:B19"/>
-    <mergeCell ref="A20:A21"/>
-    <mergeCell ref="B20:B21"/>
-    <mergeCell ref="A22:A23"/>
-    <mergeCell ref="B22:B23"/>
-    <mergeCell ref="A8:A9"/>
-    <mergeCell ref="A10:A11"/>
-    <mergeCell ref="A14:A15"/>
-    <mergeCell ref="B14:B15"/>
-    <mergeCell ref="A16:A17"/>
-    <mergeCell ref="B16:B17"/>
-    <mergeCell ref="A12:A13"/>
+    <mergeCell ref="A48:A49"/>
   </mergeCells>
   <pageMargins left="0.25" right="0.25" top="0.75" bottom="0.75" header="0" footer="0"/>
   <pageSetup scale="86" orientation="portrait"/>
@@ -8154,8 +8154,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:AK1000"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="AC5" sqref="AC5"/>
+    <sheetView tabSelected="1" topLeftCell="A19" workbookViewId="0">
+      <selection activeCell="B32" sqref="B32:B33"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="12.625" defaultRowHeight="15" customHeight="1"/>
@@ -8200,12 +8200,12 @@
       <c r="X1" s="5" t="s">
         <v>1</v>
       </c>
-      <c r="Y1" s="59">
+      <c r="Y1" s="57">
         <v>2026</v>
       </c>
-      <c r="Z1" s="60"/>
-      <c r="AA1" s="60"/>
-      <c r="AB1" s="61"/>
+      <c r="Z1" s="58"/>
+      <c r="AA1" s="58"/>
+      <c r="AB1" s="59"/>
       <c r="AC1" s="6"/>
       <c r="AD1" s="4" t="s">
         <v>2</v>
@@ -8360,12 +8360,12 @@
       <c r="AB4" s="12"/>
       <c r="AC4" s="6"/>
       <c r="AD4" s="67"/>
-      <c r="AE4" s="63"/>
-      <c r="AF4" s="63"/>
-      <c r="AG4" s="63"/>
-      <c r="AH4" s="63"/>
-      <c r="AI4" s="63"/>
-      <c r="AJ4" s="63"/>
+      <c r="AE4" s="61"/>
+      <c r="AF4" s="61"/>
+      <c r="AG4" s="61"/>
+      <c r="AH4" s="61"/>
+      <c r="AI4" s="61"/>
+      <c r="AJ4" s="61"/>
       <c r="AK4" s="68"/>
     </row>
     <row r="5" spans="1:37" ht="14.25" customHeight="1">
@@ -8413,16 +8413,16 @@
       <c r="AB5" s="16"/>
       <c r="AC5" s="6"/>
       <c r="AD5" s="67"/>
-      <c r="AE5" s="63"/>
-      <c r="AF5" s="63"/>
-      <c r="AG5" s="63"/>
-      <c r="AH5" s="63"/>
-      <c r="AI5" s="63"/>
-      <c r="AJ5" s="63"/>
+      <c r="AE5" s="61"/>
+      <c r="AF5" s="61"/>
+      <c r="AG5" s="61"/>
+      <c r="AH5" s="61"/>
+      <c r="AI5" s="61"/>
+      <c r="AJ5" s="61"/>
       <c r="AK5" s="68"/>
     </row>
     <row r="6" spans="1:37" ht="14.25" customHeight="1">
-      <c r="A6" s="54" t="s">
+      <c r="A6" s="56" t="s">
         <v>63</v>
       </c>
       <c r="B6" s="86" t="s">
@@ -8458,12 +8458,12 @@
       <c r="AB6" s="17"/>
       <c r="AC6" s="6"/>
       <c r="AD6" s="67"/>
-      <c r="AE6" s="63"/>
-      <c r="AF6" s="63"/>
-      <c r="AG6" s="63"/>
-      <c r="AH6" s="63"/>
-      <c r="AI6" s="63"/>
-      <c r="AJ6" s="63"/>
+      <c r="AE6" s="61"/>
+      <c r="AF6" s="61"/>
+      <c r="AG6" s="61"/>
+      <c r="AH6" s="61"/>
+      <c r="AI6" s="61"/>
+      <c r="AJ6" s="61"/>
       <c r="AK6" s="68"/>
     </row>
     <row r="7" spans="1:37" ht="14.25" customHeight="1">
@@ -8505,16 +8505,16 @@
       <c r="AB7" s="17"/>
       <c r="AC7" s="6"/>
       <c r="AD7" s="67"/>
-      <c r="AE7" s="63"/>
-      <c r="AF7" s="63"/>
-      <c r="AG7" s="63"/>
-      <c r="AH7" s="63"/>
-      <c r="AI7" s="63"/>
-      <c r="AJ7" s="63"/>
+      <c r="AE7" s="61"/>
+      <c r="AF7" s="61"/>
+      <c r="AG7" s="61"/>
+      <c r="AH7" s="61"/>
+      <c r="AI7" s="61"/>
+      <c r="AJ7" s="61"/>
       <c r="AK7" s="68"/>
     </row>
     <row r="8" spans="1:37" ht="14.25" customHeight="1">
-      <c r="A8" s="54" t="s">
+      <c r="A8" s="56" t="s">
         <v>52</v>
       </c>
       <c r="B8" s="84" t="s">
@@ -8550,12 +8550,12 @@
       <c r="AB8" s="17"/>
       <c r="AC8" s="6"/>
       <c r="AD8" s="67"/>
-      <c r="AE8" s="63"/>
-      <c r="AF8" s="63"/>
-      <c r="AG8" s="63"/>
-      <c r="AH8" s="63"/>
-      <c r="AI8" s="63"/>
-      <c r="AJ8" s="63"/>
+      <c r="AE8" s="61"/>
+      <c r="AF8" s="61"/>
+      <c r="AG8" s="61"/>
+      <c r="AH8" s="61"/>
+      <c r="AI8" s="61"/>
+      <c r="AJ8" s="61"/>
       <c r="AK8" s="68"/>
     </row>
     <row r="9" spans="1:37" ht="14.25" customHeight="1">
@@ -8572,7 +8572,7 @@
       </c>
       <c r="H9" s="40"/>
       <c r="I9" s="40"/>
-      <c r="J9" s="17"/>
+      <c r="J9" s="40"/>
       <c r="K9" s="17"/>
       <c r="L9" s="18"/>
       <c r="M9" s="18"/>
@@ -8593,16 +8593,16 @@
       <c r="AB9" s="17"/>
       <c r="AC9" s="6"/>
       <c r="AD9" s="67"/>
-      <c r="AE9" s="63"/>
-      <c r="AF9" s="63"/>
-      <c r="AG9" s="63"/>
-      <c r="AH9" s="63"/>
-      <c r="AI9" s="63"/>
-      <c r="AJ9" s="63"/>
+      <c r="AE9" s="61"/>
+      <c r="AF9" s="61"/>
+      <c r="AG9" s="61"/>
+      <c r="AH9" s="61"/>
+      <c r="AI9" s="61"/>
+      <c r="AJ9" s="61"/>
       <c r="AK9" s="68"/>
     </row>
     <row r="10" spans="1:37" ht="14.25" customHeight="1">
-      <c r="A10" s="54" t="s">
+      <c r="A10" s="56" t="s">
         <v>53</v>
       </c>
       <c r="B10" s="84" t="s">
@@ -8638,12 +8638,12 @@
       <c r="AB10" s="17"/>
       <c r="AC10" s="6"/>
       <c r="AD10" s="67"/>
-      <c r="AE10" s="63"/>
-      <c r="AF10" s="63"/>
-      <c r="AG10" s="63"/>
-      <c r="AH10" s="63"/>
-      <c r="AI10" s="63"/>
-      <c r="AJ10" s="63"/>
+      <c r="AE10" s="61"/>
+      <c r="AF10" s="61"/>
+      <c r="AG10" s="61"/>
+      <c r="AH10" s="61"/>
+      <c r="AI10" s="61"/>
+      <c r="AJ10" s="61"/>
       <c r="AK10" s="68"/>
     </row>
     <row r="11" spans="1:37" ht="14.25" customHeight="1">
@@ -8660,7 +8660,7 @@
       </c>
       <c r="H11" s="17"/>
       <c r="I11" s="40"/>
-      <c r="J11" s="17"/>
+      <c r="J11" s="40"/>
       <c r="K11" s="17"/>
       <c r="L11" s="18"/>
       <c r="M11" s="18"/>
@@ -8681,16 +8681,16 @@
       <c r="AB11" s="17"/>
       <c r="AC11" s="6"/>
       <c r="AD11" s="67"/>
-      <c r="AE11" s="63"/>
-      <c r="AF11" s="63"/>
-      <c r="AG11" s="63"/>
-      <c r="AH11" s="63"/>
-      <c r="AI11" s="63"/>
-      <c r="AJ11" s="63"/>
+      <c r="AE11" s="61"/>
+      <c r="AF11" s="61"/>
+      <c r="AG11" s="61"/>
+      <c r="AH11" s="61"/>
+      <c r="AI11" s="61"/>
+      <c r="AJ11" s="61"/>
       <c r="AK11" s="68"/>
     </row>
     <row r="12" spans="1:37" ht="14.25" customHeight="1">
-      <c r="A12" s="54" t="s">
+      <c r="A12" s="56" t="s">
         <v>54</v>
       </c>
       <c r="B12" s="84" t="s">
@@ -8726,12 +8726,12 @@
       <c r="AB12" s="17"/>
       <c r="AC12" s="6"/>
       <c r="AD12" s="67"/>
-      <c r="AE12" s="63"/>
-      <c r="AF12" s="63"/>
-      <c r="AG12" s="63"/>
-      <c r="AH12" s="63"/>
-      <c r="AI12" s="63"/>
-      <c r="AJ12" s="63"/>
+      <c r="AE12" s="61"/>
+      <c r="AF12" s="61"/>
+      <c r="AG12" s="61"/>
+      <c r="AH12" s="61"/>
+      <c r="AI12" s="61"/>
+      <c r="AJ12" s="61"/>
       <c r="AK12" s="68"/>
     </row>
     <row r="13" spans="1:37" ht="17.25" customHeight="1">
@@ -8748,7 +8748,7 @@
       </c>
       <c r="H13" s="17"/>
       <c r="I13" s="40"/>
-      <c r="J13" s="17"/>
+      <c r="J13" s="40"/>
       <c r="K13" s="17"/>
       <c r="L13" s="18"/>
       <c r="M13" s="18"/>
@@ -8769,16 +8769,16 @@
       <c r="AB13" s="17"/>
       <c r="AC13" s="6"/>
       <c r="AD13" s="67"/>
-      <c r="AE13" s="63"/>
-      <c r="AF13" s="63"/>
-      <c r="AG13" s="63"/>
-      <c r="AH13" s="63"/>
-      <c r="AI13" s="63"/>
-      <c r="AJ13" s="63"/>
+      <c r="AE13" s="61"/>
+      <c r="AF13" s="61"/>
+      <c r="AG13" s="61"/>
+      <c r="AH13" s="61"/>
+      <c r="AI13" s="61"/>
+      <c r="AJ13" s="61"/>
       <c r="AK13" s="68"/>
     </row>
     <row r="14" spans="1:37" ht="14.25" customHeight="1">
-      <c r="A14" s="54" t="s">
+      <c r="A14" s="56" t="s">
         <v>55</v>
       </c>
       <c r="B14" s="84" t="s">
@@ -8814,12 +8814,12 @@
       <c r="AB14" s="17"/>
       <c r="AC14" s="6"/>
       <c r="AD14" s="67"/>
-      <c r="AE14" s="63"/>
-      <c r="AF14" s="63"/>
-      <c r="AG14" s="63"/>
-      <c r="AH14" s="63"/>
-      <c r="AI14" s="63"/>
-      <c r="AJ14" s="63"/>
+      <c r="AE14" s="61"/>
+      <c r="AF14" s="61"/>
+      <c r="AG14" s="61"/>
+      <c r="AH14" s="61"/>
+      <c r="AI14" s="61"/>
+      <c r="AJ14" s="61"/>
       <c r="AK14" s="68"/>
     </row>
     <row r="15" spans="1:37" ht="17.25" customHeight="1">
@@ -8836,7 +8836,7 @@
       </c>
       <c r="H15" s="17"/>
       <c r="I15" s="40"/>
-      <c r="J15" s="17"/>
+      <c r="J15" s="40"/>
       <c r="K15" s="17"/>
       <c r="L15" s="18"/>
       <c r="M15" s="18"/>
@@ -8857,16 +8857,16 @@
       <c r="AB15" s="17"/>
       <c r="AC15" s="6"/>
       <c r="AD15" s="67"/>
-      <c r="AE15" s="63"/>
-      <c r="AF15" s="63"/>
-      <c r="AG15" s="63"/>
-      <c r="AH15" s="63"/>
-      <c r="AI15" s="63"/>
-      <c r="AJ15" s="63"/>
+      <c r="AE15" s="61"/>
+      <c r="AF15" s="61"/>
+      <c r="AG15" s="61"/>
+      <c r="AH15" s="61"/>
+      <c r="AI15" s="61"/>
+      <c r="AJ15" s="61"/>
       <c r="AK15" s="68"/>
     </row>
     <row r="16" spans="1:37" ht="14.25" customHeight="1">
-      <c r="A16" s="54" t="s">
+      <c r="A16" s="56" t="s">
         <v>56</v>
       </c>
       <c r="B16" s="84" t="s">
@@ -8902,12 +8902,12 @@
       <c r="AB16" s="17"/>
       <c r="AC16" s="6"/>
       <c r="AD16" s="67"/>
-      <c r="AE16" s="63"/>
-      <c r="AF16" s="63"/>
-      <c r="AG16" s="63"/>
-      <c r="AH16" s="63"/>
-      <c r="AI16" s="63"/>
-      <c r="AJ16" s="63"/>
+      <c r="AE16" s="61"/>
+      <c r="AF16" s="61"/>
+      <c r="AG16" s="61"/>
+      <c r="AH16" s="61"/>
+      <c r="AI16" s="61"/>
+      <c r="AJ16" s="61"/>
       <c r="AK16" s="68"/>
     </row>
     <row r="17" spans="1:37" ht="17.25" customHeight="1">
@@ -8945,16 +8945,16 @@
       <c r="AB17" s="17"/>
       <c r="AC17" s="6"/>
       <c r="AD17" s="67"/>
-      <c r="AE17" s="63"/>
-      <c r="AF17" s="63"/>
-      <c r="AG17" s="63"/>
-      <c r="AH17" s="63"/>
-      <c r="AI17" s="63"/>
-      <c r="AJ17" s="63"/>
+      <c r="AE17" s="61"/>
+      <c r="AF17" s="61"/>
+      <c r="AG17" s="61"/>
+      <c r="AH17" s="61"/>
+      <c r="AI17" s="61"/>
+      <c r="AJ17" s="61"/>
       <c r="AK17" s="68"/>
     </row>
     <row r="18" spans="1:37" ht="14.25" customHeight="1">
-      <c r="A18" s="54" t="s">
+      <c r="A18" s="56" t="s">
         <v>58</v>
       </c>
       <c r="B18" s="85" t="s">
@@ -8990,12 +8990,12 @@
       <c r="AB18" s="17"/>
       <c r="AC18" s="6"/>
       <c r="AD18" s="67"/>
-      <c r="AE18" s="63"/>
-      <c r="AF18" s="63"/>
-      <c r="AG18" s="63"/>
-      <c r="AH18" s="63"/>
-      <c r="AI18" s="63"/>
-      <c r="AJ18" s="63"/>
+      <c r="AE18" s="61"/>
+      <c r="AF18" s="61"/>
+      <c r="AG18" s="61"/>
+      <c r="AH18" s="61"/>
+      <c r="AI18" s="61"/>
+      <c r="AJ18" s="61"/>
       <c r="AK18" s="68"/>
     </row>
     <row r="19" spans="1:37" ht="14.25" customHeight="1">
@@ -9033,16 +9033,16 @@
       <c r="AB19" s="17"/>
       <c r="AC19" s="6"/>
       <c r="AD19" s="67"/>
-      <c r="AE19" s="63"/>
-      <c r="AF19" s="63"/>
-      <c r="AG19" s="63"/>
-      <c r="AH19" s="63"/>
-      <c r="AI19" s="63"/>
-      <c r="AJ19" s="63"/>
+      <c r="AE19" s="61"/>
+      <c r="AF19" s="61"/>
+      <c r="AG19" s="61"/>
+      <c r="AH19" s="61"/>
+      <c r="AI19" s="61"/>
+      <c r="AJ19" s="61"/>
       <c r="AK19" s="68"/>
     </row>
     <row r="20" spans="1:37" ht="14.25" customHeight="1">
-      <c r="A20" s="54" t="s">
+      <c r="A20" s="56" t="s">
         <v>72</v>
       </c>
       <c r="B20" s="85" t="s">
@@ -9078,12 +9078,12 @@
       <c r="AB20" s="17"/>
       <c r="AC20" s="6"/>
       <c r="AD20" s="67"/>
-      <c r="AE20" s="63"/>
-      <c r="AF20" s="63"/>
-      <c r="AG20" s="63"/>
-      <c r="AH20" s="63"/>
-      <c r="AI20" s="63"/>
-      <c r="AJ20" s="63"/>
+      <c r="AE20" s="61"/>
+      <c r="AF20" s="61"/>
+      <c r="AG20" s="61"/>
+      <c r="AH20" s="61"/>
+      <c r="AI20" s="61"/>
+      <c r="AJ20" s="61"/>
       <c r="AK20" s="68"/>
     </row>
     <row r="21" spans="1:37" ht="14.25" customHeight="1">
@@ -9100,7 +9100,7 @@
       </c>
       <c r="H21" s="17"/>
       <c r="I21" s="17"/>
-      <c r="J21" s="17"/>
+      <c r="J21" s="40"/>
       <c r="K21" s="17"/>
       <c r="L21" s="28"/>
       <c r="M21" s="28"/>
@@ -9121,16 +9121,16 @@
       <c r="AB21" s="17"/>
       <c r="AC21" s="6"/>
       <c r="AD21" s="67"/>
-      <c r="AE21" s="63"/>
-      <c r="AF21" s="63"/>
-      <c r="AG21" s="63"/>
-      <c r="AH21" s="63"/>
-      <c r="AI21" s="63"/>
-      <c r="AJ21" s="63"/>
+      <c r="AE21" s="61"/>
+      <c r="AF21" s="61"/>
+      <c r="AG21" s="61"/>
+      <c r="AH21" s="61"/>
+      <c r="AI21" s="61"/>
+      <c r="AJ21" s="61"/>
       <c r="AK21" s="68"/>
     </row>
     <row r="22" spans="1:37" ht="14.25" customHeight="1">
-      <c r="A22" s="54" t="s">
+      <c r="A22" s="56" t="s">
         <v>74</v>
       </c>
       <c r="B22" s="84" t="s">
@@ -9166,12 +9166,12 @@
       <c r="AB22" s="17"/>
       <c r="AC22" s="6"/>
       <c r="AD22" s="67"/>
-      <c r="AE22" s="63"/>
-      <c r="AF22" s="63"/>
-      <c r="AG22" s="63"/>
-      <c r="AH22" s="63"/>
-      <c r="AI22" s="63"/>
-      <c r="AJ22" s="63"/>
+      <c r="AE22" s="61"/>
+      <c r="AF22" s="61"/>
+      <c r="AG22" s="61"/>
+      <c r="AH22" s="61"/>
+      <c r="AI22" s="61"/>
+      <c r="AJ22" s="61"/>
       <c r="AK22" s="68"/>
     </row>
     <row r="23" spans="1:37" ht="14.25" customHeight="1">
@@ -9188,7 +9188,7 @@
       </c>
       <c r="H23" s="17"/>
       <c r="I23" s="17"/>
-      <c r="J23" s="17"/>
+      <c r="J23" s="40"/>
       <c r="K23" s="17"/>
       <c r="L23" s="31"/>
       <c r="M23" s="31"/>
@@ -9209,16 +9209,16 @@
       <c r="AB23" s="17"/>
       <c r="AC23" s="6"/>
       <c r="AD23" s="67"/>
-      <c r="AE23" s="63"/>
-      <c r="AF23" s="63"/>
-      <c r="AG23" s="63"/>
-      <c r="AH23" s="63"/>
-      <c r="AI23" s="63"/>
-      <c r="AJ23" s="63"/>
+      <c r="AE23" s="61"/>
+      <c r="AF23" s="61"/>
+      <c r="AG23" s="61"/>
+      <c r="AH23" s="61"/>
+      <c r="AI23" s="61"/>
+      <c r="AJ23" s="61"/>
       <c r="AK23" s="68"/>
     </row>
     <row r="24" spans="1:37" ht="14.25" customHeight="1">
-      <c r="A24" s="54" t="s">
+      <c r="A24" s="56" t="s">
         <v>76</v>
       </c>
       <c r="B24" s="85" t="s">
@@ -9254,12 +9254,12 @@
       <c r="AB24" s="17"/>
       <c r="AC24" s="6"/>
       <c r="AD24" s="67"/>
-      <c r="AE24" s="63"/>
-      <c r="AF24" s="63"/>
-      <c r="AG24" s="63"/>
-      <c r="AH24" s="63"/>
-      <c r="AI24" s="63"/>
-      <c r="AJ24" s="63"/>
+      <c r="AE24" s="61"/>
+      <c r="AF24" s="61"/>
+      <c r="AG24" s="61"/>
+      <c r="AH24" s="61"/>
+      <c r="AI24" s="61"/>
+      <c r="AJ24" s="61"/>
       <c r="AK24" s="68"/>
     </row>
     <row r="25" spans="1:37" ht="14.25" customHeight="1">
@@ -9297,16 +9297,16 @@
       <c r="AB25" s="17"/>
       <c r="AC25" s="6"/>
       <c r="AD25" s="67"/>
-      <c r="AE25" s="63"/>
-      <c r="AF25" s="63"/>
-      <c r="AG25" s="63"/>
-      <c r="AH25" s="63"/>
-      <c r="AI25" s="63"/>
-      <c r="AJ25" s="63"/>
+      <c r="AE25" s="61"/>
+      <c r="AF25" s="61"/>
+      <c r="AG25" s="61"/>
+      <c r="AH25" s="61"/>
+      <c r="AI25" s="61"/>
+      <c r="AJ25" s="61"/>
       <c r="AK25" s="68"/>
     </row>
     <row r="26" spans="1:37" ht="14.25" customHeight="1">
-      <c r="A26" s="54" t="s">
+      <c r="A26" s="56" t="s">
         <v>78</v>
       </c>
       <c r="B26" s="84" t="s">
@@ -9342,12 +9342,12 @@
       <c r="AB26" s="17"/>
       <c r="AC26" s="6"/>
       <c r="AD26" s="67"/>
-      <c r="AE26" s="63"/>
-      <c r="AF26" s="63"/>
-      <c r="AG26" s="63"/>
-      <c r="AH26" s="63"/>
-      <c r="AI26" s="63"/>
-      <c r="AJ26" s="63"/>
+      <c r="AE26" s="61"/>
+      <c r="AF26" s="61"/>
+      <c r="AG26" s="61"/>
+      <c r="AH26" s="61"/>
+      <c r="AI26" s="61"/>
+      <c r="AJ26" s="61"/>
       <c r="AK26" s="68"/>
     </row>
     <row r="27" spans="1:37" ht="17.25" customHeight="1">
@@ -9385,16 +9385,16 @@
       <c r="AB27" s="17"/>
       <c r="AC27" s="6"/>
       <c r="AD27" s="67"/>
-      <c r="AE27" s="63"/>
-      <c r="AF27" s="63"/>
-      <c r="AG27" s="63"/>
-      <c r="AH27" s="63"/>
-      <c r="AI27" s="63"/>
-      <c r="AJ27" s="63"/>
+      <c r="AE27" s="61"/>
+      <c r="AF27" s="61"/>
+      <c r="AG27" s="61"/>
+      <c r="AH27" s="61"/>
+      <c r="AI27" s="61"/>
+      <c r="AJ27" s="61"/>
       <c r="AK27" s="68"/>
     </row>
     <row r="28" spans="1:37" ht="14.25" customHeight="1">
-      <c r="A28" s="54" t="s">
+      <c r="A28" s="56" t="s">
         <v>79</v>
       </c>
       <c r="B28" s="85" t="s">
@@ -9430,12 +9430,12 @@
       <c r="AB28" s="17"/>
       <c r="AC28" s="6"/>
       <c r="AD28" s="67"/>
-      <c r="AE28" s="63"/>
-      <c r="AF28" s="63"/>
-      <c r="AG28" s="63"/>
-      <c r="AH28" s="63"/>
-      <c r="AI28" s="63"/>
-      <c r="AJ28" s="63"/>
+      <c r="AE28" s="61"/>
+      <c r="AF28" s="61"/>
+      <c r="AG28" s="61"/>
+      <c r="AH28" s="61"/>
+      <c r="AI28" s="61"/>
+      <c r="AJ28" s="61"/>
       <c r="AK28" s="68"/>
     </row>
     <row r="29" spans="1:37" ht="14.25" customHeight="1">
@@ -9473,16 +9473,16 @@
       <c r="AB29" s="17"/>
       <c r="AC29" s="6"/>
       <c r="AD29" s="67"/>
-      <c r="AE29" s="63"/>
-      <c r="AF29" s="63"/>
-      <c r="AG29" s="63"/>
-      <c r="AH29" s="63"/>
-      <c r="AI29" s="63"/>
-      <c r="AJ29" s="63"/>
+      <c r="AE29" s="61"/>
+      <c r="AF29" s="61"/>
+      <c r="AG29" s="61"/>
+      <c r="AH29" s="61"/>
+      <c r="AI29" s="61"/>
+      <c r="AJ29" s="61"/>
       <c r="AK29" s="68"/>
     </row>
     <row r="30" spans="1:37" ht="14.25" customHeight="1">
-      <c r="A30" s="54" t="s">
+      <c r="A30" s="56" t="s">
         <v>81</v>
       </c>
       <c r="B30" s="84" t="s">
@@ -9518,12 +9518,12 @@
       <c r="AB30" s="17"/>
       <c r="AC30" s="6"/>
       <c r="AD30" s="67"/>
-      <c r="AE30" s="63"/>
-      <c r="AF30" s="63"/>
-      <c r="AG30" s="63"/>
-      <c r="AH30" s="63"/>
-      <c r="AI30" s="63"/>
-      <c r="AJ30" s="63"/>
+      <c r="AE30" s="61"/>
+      <c r="AF30" s="61"/>
+      <c r="AG30" s="61"/>
+      <c r="AH30" s="61"/>
+      <c r="AI30" s="61"/>
+      <c r="AJ30" s="61"/>
       <c r="AK30" s="68"/>
     </row>
     <row r="31" spans="1:37" ht="14.25" customHeight="1">
@@ -9570,7 +9570,7 @@
       <c r="AK31" s="71"/>
     </row>
     <row r="32" spans="1:37" ht="14.25" customHeight="1">
-      <c r="A32" s="54" t="s">
+      <c r="A32" s="56" t="s">
         <v>82</v>
       </c>
       <c r="B32" s="85" t="s">
@@ -9658,7 +9658,7 @@
       <c r="AK33" s="52"/>
     </row>
     <row r="34" spans="1:37" ht="14.25" customHeight="1">
-      <c r="A34" s="54" t="s">
+      <c r="A34" s="56" t="s">
         <v>84</v>
       </c>
       <c r="B34" s="84" t="s">
@@ -9737,16 +9737,16 @@
       <c r="AB35" s="17"/>
       <c r="AC35" s="6"/>
       <c r="AD35" s="76"/>
-      <c r="AE35" s="63"/>
-      <c r="AF35" s="63"/>
-      <c r="AG35" s="63"/>
-      <c r="AH35" s="63"/>
-      <c r="AI35" s="63"/>
-      <c r="AJ35" s="63"/>
+      <c r="AE35" s="61"/>
+      <c r="AF35" s="61"/>
+      <c r="AG35" s="61"/>
+      <c r="AH35" s="61"/>
+      <c r="AI35" s="61"/>
+      <c r="AJ35" s="61"/>
       <c r="AK35" s="77"/>
     </row>
     <row r="36" spans="1:37" ht="14.25" customHeight="1">
-      <c r="A36" s="54" t="s">
+      <c r="A36" s="56" t="s">
         <v>85</v>
       </c>
       <c r="B36" s="85" t="s">
@@ -9782,12 +9782,12 @@
       <c r="AB36" s="17"/>
       <c r="AC36" s="6"/>
       <c r="AD36" s="76"/>
-      <c r="AE36" s="63"/>
-      <c r="AF36" s="63"/>
-      <c r="AG36" s="63"/>
-      <c r="AH36" s="63"/>
-      <c r="AI36" s="63"/>
-      <c r="AJ36" s="63"/>
+      <c r="AE36" s="61"/>
+      <c r="AF36" s="61"/>
+      <c r="AG36" s="61"/>
+      <c r="AH36" s="61"/>
+      <c r="AI36" s="61"/>
+      <c r="AJ36" s="61"/>
       <c r="AK36" s="77"/>
     </row>
     <row r="37" spans="1:37" ht="14.25" customHeight="1">
@@ -9825,16 +9825,16 @@
       <c r="AB37" s="17"/>
       <c r="AC37" s="6"/>
       <c r="AD37" s="76"/>
-      <c r="AE37" s="63"/>
-      <c r="AF37" s="63"/>
-      <c r="AG37" s="63"/>
-      <c r="AH37" s="63"/>
-      <c r="AI37" s="63"/>
-      <c r="AJ37" s="63"/>
+      <c r="AE37" s="61"/>
+      <c r="AF37" s="61"/>
+      <c r="AG37" s="61"/>
+      <c r="AH37" s="61"/>
+      <c r="AI37" s="61"/>
+      <c r="AJ37" s="61"/>
       <c r="AK37" s="77"/>
     </row>
     <row r="38" spans="1:37" ht="14.25" customHeight="1">
-      <c r="A38" s="54" t="s">
+      <c r="A38" s="56" t="s">
         <v>86</v>
       </c>
       <c r="B38" s="84" t="s">
@@ -9870,12 +9870,12 @@
       <c r="AB38" s="17"/>
       <c r="AC38" s="6"/>
       <c r="AD38" s="76"/>
-      <c r="AE38" s="63"/>
-      <c r="AF38" s="63"/>
-      <c r="AG38" s="63"/>
-      <c r="AH38" s="63"/>
-      <c r="AI38" s="63"/>
-      <c r="AJ38" s="63"/>
+      <c r="AE38" s="61"/>
+      <c r="AF38" s="61"/>
+      <c r="AG38" s="61"/>
+      <c r="AH38" s="61"/>
+      <c r="AI38" s="61"/>
+      <c r="AJ38" s="61"/>
       <c r="AK38" s="77"/>
     </row>
     <row r="39" spans="1:37" ht="14.25" customHeight="1">
@@ -9913,16 +9913,16 @@
       <c r="AB39" s="17"/>
       <c r="AC39" s="6"/>
       <c r="AD39" s="76"/>
-      <c r="AE39" s="63"/>
-      <c r="AF39" s="63"/>
-      <c r="AG39" s="63"/>
-      <c r="AH39" s="63"/>
-      <c r="AI39" s="63"/>
-      <c r="AJ39" s="63"/>
+      <c r="AE39" s="61"/>
+      <c r="AF39" s="61"/>
+      <c r="AG39" s="61"/>
+      <c r="AH39" s="61"/>
+      <c r="AI39" s="61"/>
+      <c r="AJ39" s="61"/>
       <c r="AK39" s="77"/>
     </row>
     <row r="40" spans="1:37" ht="15" customHeight="1">
-      <c r="A40" s="54" t="s">
+      <c r="A40" s="56" t="s">
         <v>87</v>
       </c>
       <c r="B40" s="85" t="s">
@@ -9958,12 +9958,12 @@
       <c r="AB40" s="17"/>
       <c r="AC40" s="6"/>
       <c r="AD40" s="76"/>
-      <c r="AE40" s="63"/>
-      <c r="AF40" s="63"/>
-      <c r="AG40" s="63"/>
-      <c r="AH40" s="63"/>
-      <c r="AI40" s="63"/>
-      <c r="AJ40" s="63"/>
+      <c r="AE40" s="61"/>
+      <c r="AF40" s="61"/>
+      <c r="AG40" s="61"/>
+      <c r="AH40" s="61"/>
+      <c r="AI40" s="61"/>
+      <c r="AJ40" s="61"/>
       <c r="AK40" s="77"/>
     </row>
     <row r="41" spans="1:37" ht="15" customHeight="1">
@@ -10001,16 +10001,16 @@
       <c r="AB41" s="17"/>
       <c r="AC41" s="6"/>
       <c r="AD41" s="76"/>
-      <c r="AE41" s="63"/>
-      <c r="AF41" s="63"/>
-      <c r="AG41" s="63"/>
-      <c r="AH41" s="63"/>
-      <c r="AI41" s="63"/>
-      <c r="AJ41" s="63"/>
+      <c r="AE41" s="61"/>
+      <c r="AF41" s="61"/>
+      <c r="AG41" s="61"/>
+      <c r="AH41" s="61"/>
+      <c r="AI41" s="61"/>
+      <c r="AJ41" s="61"/>
       <c r="AK41" s="77"/>
     </row>
     <row r="42" spans="1:37" ht="15" customHeight="1">
-      <c r="A42" s="54" t="s">
+      <c r="A42" s="56" t="s">
         <v>88</v>
       </c>
       <c r="B42" s="84" t="s">
@@ -10046,12 +10046,12 @@
       <c r="AB42" s="17"/>
       <c r="AC42" s="6"/>
       <c r="AD42" s="76"/>
-      <c r="AE42" s="63"/>
-      <c r="AF42" s="63"/>
-      <c r="AG42" s="63"/>
-      <c r="AH42" s="63"/>
-      <c r="AI42" s="63"/>
-      <c r="AJ42" s="63"/>
+      <c r="AE42" s="61"/>
+      <c r="AF42" s="61"/>
+      <c r="AG42" s="61"/>
+      <c r="AH42" s="61"/>
+      <c r="AI42" s="61"/>
+      <c r="AJ42" s="61"/>
       <c r="AK42" s="77"/>
     </row>
     <row r="43" spans="1:37" ht="15" customHeight="1">
@@ -10089,16 +10089,16 @@
       <c r="AB43" s="17"/>
       <c r="AC43" s="6"/>
       <c r="AD43" s="76"/>
-      <c r="AE43" s="63"/>
-      <c r="AF43" s="63"/>
-      <c r="AG43" s="63"/>
-      <c r="AH43" s="63"/>
-      <c r="AI43" s="63"/>
-      <c r="AJ43" s="63"/>
+      <c r="AE43" s="61"/>
+      <c r="AF43" s="61"/>
+      <c r="AG43" s="61"/>
+      <c r="AH43" s="61"/>
+      <c r="AI43" s="61"/>
+      <c r="AJ43" s="61"/>
       <c r="AK43" s="77"/>
     </row>
     <row r="44" spans="1:37" ht="14.25" customHeight="1">
-      <c r="A44" s="54" t="s">
+      <c r="A44" s="56" t="s">
         <v>89</v>
       </c>
       <c r="B44" s="85" t="s">
@@ -10134,12 +10134,12 @@
       <c r="AB44" s="17"/>
       <c r="AC44" s="6"/>
       <c r="AD44" s="76"/>
-      <c r="AE44" s="63"/>
-      <c r="AF44" s="63"/>
-      <c r="AG44" s="63"/>
-      <c r="AH44" s="63"/>
-      <c r="AI44" s="63"/>
-      <c r="AJ44" s="63"/>
+      <c r="AE44" s="61"/>
+      <c r="AF44" s="61"/>
+      <c r="AG44" s="61"/>
+      <c r="AH44" s="61"/>
+      <c r="AI44" s="61"/>
+      <c r="AJ44" s="61"/>
       <c r="AK44" s="77"/>
     </row>
     <row r="45" spans="1:37" ht="14.25" customHeight="1">
@@ -10177,16 +10177,16 @@
       <c r="AB45" s="17"/>
       <c r="AC45" s="6"/>
       <c r="AD45" s="76"/>
-      <c r="AE45" s="63"/>
-      <c r="AF45" s="63"/>
-      <c r="AG45" s="63"/>
-      <c r="AH45" s="63"/>
-      <c r="AI45" s="63"/>
-      <c r="AJ45" s="63"/>
+      <c r="AE45" s="61"/>
+      <c r="AF45" s="61"/>
+      <c r="AG45" s="61"/>
+      <c r="AH45" s="61"/>
+      <c r="AI45" s="61"/>
+      <c r="AJ45" s="61"/>
       <c r="AK45" s="77"/>
     </row>
     <row r="46" spans="1:37" ht="14.25" customHeight="1">
-      <c r="A46" s="54" t="s">
+      <c r="A46" s="56" t="s">
         <v>91</v>
       </c>
       <c r="B46" s="84" t="s">
@@ -10222,12 +10222,12 @@
       <c r="AB46" s="17"/>
       <c r="AC46" s="6"/>
       <c r="AD46" s="76"/>
-      <c r="AE46" s="63"/>
-      <c r="AF46" s="63"/>
-      <c r="AG46" s="63"/>
-      <c r="AH46" s="63"/>
-      <c r="AI46" s="63"/>
-      <c r="AJ46" s="63"/>
+      <c r="AE46" s="61"/>
+      <c r="AF46" s="61"/>
+      <c r="AG46" s="61"/>
+      <c r="AH46" s="61"/>
+      <c r="AI46" s="61"/>
+      <c r="AJ46" s="61"/>
       <c r="AK46" s="77"/>
     </row>
     <row r="47" spans="1:37" ht="14.25" customHeight="1">
@@ -10265,16 +10265,16 @@
       <c r="AB47" s="17"/>
       <c r="AC47" s="6"/>
       <c r="AD47" s="76"/>
-      <c r="AE47" s="63"/>
-      <c r="AF47" s="63"/>
-      <c r="AG47" s="63"/>
-      <c r="AH47" s="63"/>
-      <c r="AI47" s="63"/>
-      <c r="AJ47" s="63"/>
+      <c r="AE47" s="61"/>
+      <c r="AF47" s="61"/>
+      <c r="AG47" s="61"/>
+      <c r="AH47" s="61"/>
+      <c r="AI47" s="61"/>
+      <c r="AJ47" s="61"/>
       <c r="AK47" s="77"/>
     </row>
     <row r="48" spans="1:37" ht="14.25" customHeight="1">
-      <c r="A48" s="54" t="s">
+      <c r="A48" s="56" t="s">
         <v>92</v>
       </c>
       <c r="B48" s="85" t="s">
@@ -10364,7 +10364,7 @@
       <c r="AK49" s="38"/>
     </row>
     <row r="50" spans="1:37" ht="14.25" customHeight="1">
-      <c r="A50" s="54" t="s">
+      <c r="A50" s="56" t="s">
         <v>94</v>
       </c>
       <c r="B50" s="85" t="s">
@@ -10456,7 +10456,7 @@
       <c r="AK51" s="38"/>
     </row>
     <row r="52" spans="1:37" ht="14.25" customHeight="1">
-      <c r="A52" s="54" t="s">
+      <c r="A52" s="56" t="s">
         <v>96</v>
       </c>
       <c r="B52" s="85" t="s">
@@ -10548,7 +10548,7 @@
       <c r="AK53" s="38"/>
     </row>
     <row r="54" spans="1:37" ht="14.25" customHeight="1">
-      <c r="A54" s="54" t="s">
+      <c r="A54" s="56" t="s">
         <v>98</v>
       </c>
       <c r="B54" s="85" t="s">
@@ -10638,7 +10638,7 @@
       <c r="AK55" s="38"/>
     </row>
     <row r="56" spans="1:37" ht="14.25" customHeight="1">
-      <c r="A56" s="54" t="s">
+      <c r="A56" s="56" t="s">
         <v>100</v>
       </c>
       <c r="B56" s="85" t="s">
@@ -10718,7 +10718,7 @@
       <c r="AC57" s="6"/>
     </row>
     <row r="58" spans="1:37" ht="14.25" customHeight="1">
-      <c r="A58" s="54" t="s">
+      <c r="A58" s="56" t="s">
         <v>102</v>
       </c>
       <c r="B58" s="85" t="s">
@@ -10791,7 +10791,7 @@
       <c r="AC59" s="6"/>
     </row>
     <row r="60" spans="1:37" ht="14.25" customHeight="1">
-      <c r="A60" s="54" t="s">
+      <c r="A60" s="56" t="s">
         <v>104</v>
       </c>
       <c r="B60" s="85" t="s">
@@ -10868,7 +10868,7 @@
       <c r="AC61" s="6"/>
     </row>
     <row r="62" spans="1:37" ht="14.25" customHeight="1">
-      <c r="A62" s="54" t="s">
+      <c r="A62" s="56" t="s">
         <v>106</v>
       </c>
       <c r="B62" s="85" t="s">
@@ -10942,7 +10942,7 @@
       <c r="AC63" s="6"/>
     </row>
     <row r="64" spans="1:37" ht="14.25" customHeight="1">
-      <c r="A64" s="54" t="s">
+      <c r="A64" s="56" t="s">
         <v>108</v>
       </c>
       <c r="B64" s="85" t="s">
@@ -11018,7 +11018,7 @@
       <c r="AC65" s="6"/>
     </row>
     <row r="66" spans="1:29" ht="14.25" customHeight="1">
-      <c r="A66" s="54" t="s">
+      <c r="A66" s="56" t="s">
         <v>110</v>
       </c>
       <c r="B66" s="85" t="s">
@@ -13950,22 +13950,23 @@
     <mergeCell ref="B44:B45"/>
     <mergeCell ref="A48:A49"/>
     <mergeCell ref="B48:B49"/>
+    <mergeCell ref="A36:A37"/>
+    <mergeCell ref="A46:A47"/>
+    <mergeCell ref="B46:B47"/>
+    <mergeCell ref="A34:A35"/>
+    <mergeCell ref="B34:B35"/>
     <mergeCell ref="AD3:AK31"/>
     <mergeCell ref="A6:A7"/>
     <mergeCell ref="B6:B7"/>
     <mergeCell ref="B8:B9"/>
     <mergeCell ref="B10:B11"/>
     <mergeCell ref="A8:A9"/>
-    <mergeCell ref="A36:A37"/>
-    <mergeCell ref="A46:A47"/>
-    <mergeCell ref="B46:B47"/>
+    <mergeCell ref="B18:B19"/>
     <mergeCell ref="Y1:AB1"/>
     <mergeCell ref="A26:A27"/>
     <mergeCell ref="B26:B27"/>
     <mergeCell ref="A32:A33"/>
     <mergeCell ref="B32:B33"/>
-    <mergeCell ref="A34:A35"/>
-    <mergeCell ref="B34:B35"/>
     <mergeCell ref="A20:A21"/>
     <mergeCell ref="B20:B21"/>
     <mergeCell ref="A22:A23"/>
@@ -13977,7 +13978,6 @@
     <mergeCell ref="A16:A17"/>
     <mergeCell ref="B16:B17"/>
     <mergeCell ref="A18:A19"/>
-    <mergeCell ref="B18:B19"/>
   </mergeCells>
   <pageMargins left="0.25" right="0.25" top="0.75" bottom="0.75" header="0" footer="0"/>
   <pageSetup scale="86" orientation="portrait"/>
@@ -14035,12 +14035,12 @@
       <c r="Z1" s="5" t="s">
         <v>1</v>
       </c>
-      <c r="AA1" s="59">
+      <c r="AA1" s="57">
         <v>2024</v>
       </c>
-      <c r="AB1" s="60"/>
-      <c r="AC1" s="60"/>
-      <c r="AD1" s="61"/>
+      <c r="AB1" s="58"/>
+      <c r="AC1" s="58"/>
+      <c r="AD1" s="59"/>
       <c r="AE1" s="6"/>
       <c r="AF1" s="4" t="s">
         <v>2</v>
@@ -14096,10 +14096,10 @@
       <c r="A3" s="11" t="s">
         <v>118</v>
       </c>
-      <c r="D3" s="62"/>
-      <c r="E3" s="63"/>
-      <c r="F3" s="63"/>
-      <c r="G3" s="63"/>
+      <c r="D3" s="60"/>
+      <c r="E3" s="61"/>
+      <c r="F3" s="61"/>
+      <c r="G3" s="61"/>
       <c r="J3" s="13" t="s">
         <v>5</v>
       </c>
@@ -14176,10 +14176,10 @@
       <c r="AM3" s="66"/>
     </row>
     <row r="4" spans="1:39" ht="14.25" customHeight="1">
-      <c r="D4" s="62"/>
-      <c r="E4" s="63"/>
-      <c r="F4" s="63"/>
-      <c r="G4" s="63"/>
+      <c r="D4" s="60"/>
+      <c r="E4" s="61"/>
+      <c r="F4" s="61"/>
+      <c r="G4" s="61"/>
       <c r="J4" s="12"/>
       <c r="K4" s="12"/>
       <c r="L4" s="12"/>
@@ -14203,12 +14203,12 @@
       <c r="AD4" s="12"/>
       <c r="AE4" s="6"/>
       <c r="AF4" s="67"/>
-      <c r="AG4" s="63"/>
-      <c r="AH4" s="63"/>
-      <c r="AI4" s="63"/>
-      <c r="AJ4" s="63"/>
-      <c r="AK4" s="63"/>
-      <c r="AL4" s="63"/>
+      <c r="AG4" s="61"/>
+      <c r="AH4" s="61"/>
+      <c r="AI4" s="61"/>
+      <c r="AJ4" s="61"/>
+      <c r="AK4" s="61"/>
+      <c r="AL4" s="61"/>
       <c r="AM4" s="68"/>
     </row>
     <row r="5" spans="1:39" ht="14.25" customHeight="1">
@@ -14262,16 +14262,16 @@
       <c r="AD5" s="16"/>
       <c r="AE5" s="6"/>
       <c r="AF5" s="67"/>
-      <c r="AG5" s="63"/>
-      <c r="AH5" s="63"/>
-      <c r="AI5" s="63"/>
-      <c r="AJ5" s="63"/>
-      <c r="AK5" s="63"/>
-      <c r="AL5" s="63"/>
+      <c r="AG5" s="61"/>
+      <c r="AH5" s="61"/>
+      <c r="AI5" s="61"/>
+      <c r="AJ5" s="61"/>
+      <c r="AK5" s="61"/>
+      <c r="AL5" s="61"/>
       <c r="AM5" s="68"/>
     </row>
     <row r="6" spans="1:39" ht="14.25" customHeight="1">
-      <c r="A6" s="54" t="s">
+      <c r="A6" s="56" t="s">
         <v>63</v>
       </c>
       <c r="B6" s="72"/>
@@ -14307,12 +14307,12 @@
       <c r="AD6" s="17"/>
       <c r="AE6" s="6"/>
       <c r="AF6" s="67"/>
-      <c r="AG6" s="63"/>
-      <c r="AH6" s="63"/>
-      <c r="AI6" s="63"/>
-      <c r="AJ6" s="63"/>
-      <c r="AK6" s="63"/>
-      <c r="AL6" s="63"/>
+      <c r="AG6" s="61"/>
+      <c r="AH6" s="61"/>
+      <c r="AI6" s="61"/>
+      <c r="AJ6" s="61"/>
+      <c r="AK6" s="61"/>
+      <c r="AL6" s="61"/>
       <c r="AM6" s="68"/>
     </row>
     <row r="7" spans="1:39" ht="14.25" customHeight="1">
@@ -14350,19 +14350,19 @@
       <c r="AD7" s="17"/>
       <c r="AE7" s="6"/>
       <c r="AF7" s="67"/>
-      <c r="AG7" s="63"/>
-      <c r="AH7" s="63"/>
-      <c r="AI7" s="63"/>
-      <c r="AJ7" s="63"/>
-      <c r="AK7" s="63"/>
-      <c r="AL7" s="63"/>
+      <c r="AG7" s="61"/>
+      <c r="AH7" s="61"/>
+      <c r="AI7" s="61"/>
+      <c r="AJ7" s="61"/>
+      <c r="AK7" s="61"/>
+      <c r="AL7" s="61"/>
       <c r="AM7" s="68"/>
     </row>
     <row r="8" spans="1:39" ht="14.25" customHeight="1">
-      <c r="A8" s="54" t="s">
+      <c r="A8" s="56" t="s">
         <v>120</v>
       </c>
-      <c r="B8" s="56"/>
+      <c r="B8" s="63"/>
       <c r="D8" s="22"/>
       <c r="E8" s="22"/>
       <c r="F8" s="22"/>
@@ -14395,12 +14395,12 @@
       <c r="AD8" s="17"/>
       <c r="AE8" s="6"/>
       <c r="AF8" s="67"/>
-      <c r="AG8" s="63"/>
-      <c r="AH8" s="63"/>
-      <c r="AI8" s="63"/>
-      <c r="AJ8" s="63"/>
-      <c r="AK8" s="63"/>
-      <c r="AL8" s="63"/>
+      <c r="AG8" s="61"/>
+      <c r="AH8" s="61"/>
+      <c r="AI8" s="61"/>
+      <c r="AJ8" s="61"/>
+      <c r="AK8" s="61"/>
+      <c r="AL8" s="61"/>
       <c r="AM8" s="68"/>
     </row>
     <row r="9" spans="1:39" ht="14.25" customHeight="1">
@@ -14438,19 +14438,19 @@
       <c r="AD9" s="17"/>
       <c r="AE9" s="6"/>
       <c r="AF9" s="67"/>
-      <c r="AG9" s="63"/>
-      <c r="AH9" s="63"/>
-      <c r="AI9" s="63"/>
-      <c r="AJ9" s="63"/>
-      <c r="AK9" s="63"/>
-      <c r="AL9" s="63"/>
+      <c r="AG9" s="61"/>
+      <c r="AH9" s="61"/>
+      <c r="AI9" s="61"/>
+      <c r="AJ9" s="61"/>
+      <c r="AK9" s="61"/>
+      <c r="AL9" s="61"/>
       <c r="AM9" s="68"/>
     </row>
     <row r="10" spans="1:39" ht="14.25" customHeight="1">
-      <c r="A10" s="54" t="s">
+      <c r="A10" s="56" t="s">
         <v>121</v>
       </c>
-      <c r="B10" s="56"/>
+      <c r="B10" s="63"/>
       <c r="D10" s="22"/>
       <c r="E10" s="22"/>
       <c r="F10" s="22"/>
@@ -14483,12 +14483,12 @@
       <c r="AD10" s="17"/>
       <c r="AE10" s="6"/>
       <c r="AF10" s="67"/>
-      <c r="AG10" s="63"/>
-      <c r="AH10" s="63"/>
-      <c r="AI10" s="63"/>
-      <c r="AJ10" s="63"/>
-      <c r="AK10" s="63"/>
-      <c r="AL10" s="63"/>
+      <c r="AG10" s="61"/>
+      <c r="AH10" s="61"/>
+      <c r="AI10" s="61"/>
+      <c r="AJ10" s="61"/>
+      <c r="AK10" s="61"/>
+      <c r="AL10" s="61"/>
       <c r="AM10" s="68"/>
     </row>
     <row r="11" spans="1:39" ht="14.25" customHeight="1">
@@ -14526,19 +14526,19 @@
       <c r="AD11" s="17"/>
       <c r="AE11" s="6"/>
       <c r="AF11" s="67"/>
-      <c r="AG11" s="63"/>
-      <c r="AH11" s="63"/>
-      <c r="AI11" s="63"/>
-      <c r="AJ11" s="63"/>
-      <c r="AK11" s="63"/>
-      <c r="AL11" s="63"/>
+      <c r="AG11" s="61"/>
+      <c r="AH11" s="61"/>
+      <c r="AI11" s="61"/>
+      <c r="AJ11" s="61"/>
+      <c r="AK11" s="61"/>
+      <c r="AL11" s="61"/>
       <c r="AM11" s="68"/>
     </row>
     <row r="12" spans="1:39" ht="14.25" customHeight="1">
-      <c r="A12" s="54" t="s">
+      <c r="A12" s="56" t="s">
         <v>122</v>
       </c>
-      <c r="B12" s="56"/>
+      <c r="B12" s="63"/>
       <c r="D12" s="22"/>
       <c r="E12" s="22"/>
       <c r="F12" s="22"/>
@@ -14571,12 +14571,12 @@
       <c r="AD12" s="17"/>
       <c r="AE12" s="6"/>
       <c r="AF12" s="67"/>
-      <c r="AG12" s="63"/>
-      <c r="AH12" s="63"/>
-      <c r="AI12" s="63"/>
-      <c r="AJ12" s="63"/>
-      <c r="AK12" s="63"/>
-      <c r="AL12" s="63"/>
+      <c r="AG12" s="61"/>
+      <c r="AH12" s="61"/>
+      <c r="AI12" s="61"/>
+      <c r="AJ12" s="61"/>
+      <c r="AK12" s="61"/>
+      <c r="AL12" s="61"/>
       <c r="AM12" s="68"/>
     </row>
     <row r="13" spans="1:39" ht="14.25" customHeight="1">
@@ -14614,19 +14614,19 @@
       <c r="AD13" s="17"/>
       <c r="AE13" s="6"/>
       <c r="AF13" s="67"/>
-      <c r="AG13" s="63"/>
-      <c r="AH13" s="63"/>
-      <c r="AI13" s="63"/>
-      <c r="AJ13" s="63"/>
-      <c r="AK13" s="63"/>
-      <c r="AL13" s="63"/>
+      <c r="AG13" s="61"/>
+      <c r="AH13" s="61"/>
+      <c r="AI13" s="61"/>
+      <c r="AJ13" s="61"/>
+      <c r="AK13" s="61"/>
+      <c r="AL13" s="61"/>
       <c r="AM13" s="68"/>
     </row>
     <row r="14" spans="1:39" ht="14.25" customHeight="1">
-      <c r="A14" s="54" t="s">
+      <c r="A14" s="56" t="s">
         <v>34</v>
       </c>
-      <c r="B14" s="56"/>
+      <c r="B14" s="63"/>
       <c r="D14" s="22"/>
       <c r="E14" s="22"/>
       <c r="F14" s="22"/>
@@ -14659,12 +14659,12 @@
       <c r="AD14" s="17"/>
       <c r="AE14" s="6"/>
       <c r="AF14" s="67"/>
-      <c r="AG14" s="63"/>
-      <c r="AH14" s="63"/>
-      <c r="AI14" s="63"/>
-      <c r="AJ14" s="63"/>
-      <c r="AK14" s="63"/>
-      <c r="AL14" s="63"/>
+      <c r="AG14" s="61"/>
+      <c r="AH14" s="61"/>
+      <c r="AI14" s="61"/>
+      <c r="AJ14" s="61"/>
+      <c r="AK14" s="61"/>
+      <c r="AL14" s="61"/>
       <c r="AM14" s="68"/>
     </row>
     <row r="15" spans="1:39" ht="17.25" customHeight="1">
@@ -14702,19 +14702,19 @@
       <c r="AD15" s="17"/>
       <c r="AE15" s="6"/>
       <c r="AF15" s="67"/>
-      <c r="AG15" s="63"/>
-      <c r="AH15" s="63"/>
-      <c r="AI15" s="63"/>
-      <c r="AJ15" s="63"/>
-      <c r="AK15" s="63"/>
-      <c r="AL15" s="63"/>
+      <c r="AG15" s="61"/>
+      <c r="AH15" s="61"/>
+      <c r="AI15" s="61"/>
+      <c r="AJ15" s="61"/>
+      <c r="AK15" s="61"/>
+      <c r="AL15" s="61"/>
       <c r="AM15" s="68"/>
     </row>
     <row r="16" spans="1:39" ht="14.25" customHeight="1">
-      <c r="A16" s="54" t="s">
+      <c r="A16" s="56" t="s">
         <v>35</v>
       </c>
-      <c r="B16" s="56"/>
+      <c r="B16" s="63"/>
       <c r="D16" s="22"/>
       <c r="E16" s="22"/>
       <c r="F16" s="22"/>
@@ -14747,12 +14747,12 @@
       <c r="AD16" s="17"/>
       <c r="AE16" s="6"/>
       <c r="AF16" s="67"/>
-      <c r="AG16" s="63"/>
-      <c r="AH16" s="63"/>
-      <c r="AI16" s="63"/>
-      <c r="AJ16" s="63"/>
-      <c r="AK16" s="63"/>
-      <c r="AL16" s="63"/>
+      <c r="AG16" s="61"/>
+      <c r="AH16" s="61"/>
+      <c r="AI16" s="61"/>
+      <c r="AJ16" s="61"/>
+      <c r="AK16" s="61"/>
+      <c r="AL16" s="61"/>
       <c r="AM16" s="68"/>
     </row>
     <row r="17" spans="1:39" ht="17.25" customHeight="1">
@@ -14790,19 +14790,19 @@
       <c r="AD17" s="17"/>
       <c r="AE17" s="6"/>
       <c r="AF17" s="67"/>
-      <c r="AG17" s="63"/>
-      <c r="AH17" s="63"/>
-      <c r="AI17" s="63"/>
-      <c r="AJ17" s="63"/>
-      <c r="AK17" s="63"/>
-      <c r="AL17" s="63"/>
+      <c r="AG17" s="61"/>
+      <c r="AH17" s="61"/>
+      <c r="AI17" s="61"/>
+      <c r="AJ17" s="61"/>
+      <c r="AK17" s="61"/>
+      <c r="AL17" s="61"/>
       <c r="AM17" s="68"/>
     </row>
     <row r="18" spans="1:39" ht="14.25" customHeight="1">
-      <c r="A18" s="54" t="s">
+      <c r="A18" s="56" t="s">
         <v>36</v>
       </c>
-      <c r="B18" s="56"/>
+      <c r="B18" s="63"/>
       <c r="D18" s="22"/>
       <c r="E18" s="22"/>
       <c r="F18" s="22"/>
@@ -14835,12 +14835,12 @@
       <c r="AD18" s="17"/>
       <c r="AE18" s="6"/>
       <c r="AF18" s="67"/>
-      <c r="AG18" s="63"/>
-      <c r="AH18" s="63"/>
-      <c r="AI18" s="63"/>
-      <c r="AJ18" s="63"/>
-      <c r="AK18" s="63"/>
-      <c r="AL18" s="63"/>
+      <c r="AG18" s="61"/>
+      <c r="AH18" s="61"/>
+      <c r="AI18" s="61"/>
+      <c r="AJ18" s="61"/>
+      <c r="AK18" s="61"/>
+      <c r="AL18" s="61"/>
       <c r="AM18" s="68"/>
     </row>
     <row r="19" spans="1:39" ht="17.25" customHeight="1">
@@ -14878,19 +14878,19 @@
       <c r="AD19" s="17"/>
       <c r="AE19" s="6"/>
       <c r="AF19" s="67"/>
-      <c r="AG19" s="63"/>
-      <c r="AH19" s="63"/>
-      <c r="AI19" s="63"/>
-      <c r="AJ19" s="63"/>
-      <c r="AK19" s="63"/>
-      <c r="AL19" s="63"/>
+      <c r="AG19" s="61"/>
+      <c r="AH19" s="61"/>
+      <c r="AI19" s="61"/>
+      <c r="AJ19" s="61"/>
+      <c r="AK19" s="61"/>
+      <c r="AL19" s="61"/>
       <c r="AM19" s="68"/>
     </row>
     <row r="20" spans="1:39" ht="14.25" customHeight="1">
-      <c r="A20" s="54" t="s">
+      <c r="A20" s="56" t="s">
         <v>37</v>
       </c>
-      <c r="B20" s="57"/>
+      <c r="B20" s="54"/>
       <c r="D20" s="22"/>
       <c r="E20" s="22"/>
       <c r="F20" s="22"/>
@@ -14923,12 +14923,12 @@
       <c r="AD20" s="17"/>
       <c r="AE20" s="6"/>
       <c r="AF20" s="67"/>
-      <c r="AG20" s="63"/>
-      <c r="AH20" s="63"/>
-      <c r="AI20" s="63"/>
-      <c r="AJ20" s="63"/>
-      <c r="AK20" s="63"/>
-      <c r="AL20" s="63"/>
+      <c r="AG20" s="61"/>
+      <c r="AH20" s="61"/>
+      <c r="AI20" s="61"/>
+      <c r="AJ20" s="61"/>
+      <c r="AK20" s="61"/>
+      <c r="AL20" s="61"/>
       <c r="AM20" s="68"/>
     </row>
     <row r="21" spans="1:39" ht="14.25" customHeight="1">
@@ -14966,19 +14966,19 @@
       <c r="AD21" s="17"/>
       <c r="AE21" s="6"/>
       <c r="AF21" s="67"/>
-      <c r="AG21" s="63"/>
-      <c r="AH21" s="63"/>
-      <c r="AI21" s="63"/>
-      <c r="AJ21" s="63"/>
-      <c r="AK21" s="63"/>
-      <c r="AL21" s="63"/>
+      <c r="AG21" s="61"/>
+      <c r="AH21" s="61"/>
+      <c r="AI21" s="61"/>
+      <c r="AJ21" s="61"/>
+      <c r="AK21" s="61"/>
+      <c r="AL21" s="61"/>
       <c r="AM21" s="68"/>
     </row>
     <row r="22" spans="1:39" ht="14.25" customHeight="1">
-      <c r="A22" s="54" t="s">
+      <c r="A22" s="56" t="s">
         <v>38</v>
       </c>
-      <c r="B22" s="57"/>
+      <c r="B22" s="54"/>
       <c r="D22" s="22"/>
       <c r="E22" s="22"/>
       <c r="F22" s="22"/>
@@ -15011,12 +15011,12 @@
       <c r="AD22" s="17"/>
       <c r="AE22" s="6"/>
       <c r="AF22" s="67"/>
-      <c r="AG22" s="63"/>
-      <c r="AH22" s="63"/>
-      <c r="AI22" s="63"/>
-      <c r="AJ22" s="63"/>
-      <c r="AK22" s="63"/>
-      <c r="AL22" s="63"/>
+      <c r="AG22" s="61"/>
+      <c r="AH22" s="61"/>
+      <c r="AI22" s="61"/>
+      <c r="AJ22" s="61"/>
+      <c r="AK22" s="61"/>
+      <c r="AL22" s="61"/>
       <c r="AM22" s="68"/>
     </row>
     <row r="23" spans="1:39" ht="14.25" customHeight="1">
@@ -15054,19 +15054,19 @@
       <c r="AD23" s="17"/>
       <c r="AE23" s="6"/>
       <c r="AF23" s="67"/>
-      <c r="AG23" s="63"/>
-      <c r="AH23" s="63"/>
-      <c r="AI23" s="63"/>
-      <c r="AJ23" s="63"/>
-      <c r="AK23" s="63"/>
-      <c r="AL23" s="63"/>
+      <c r="AG23" s="61"/>
+      <c r="AH23" s="61"/>
+      <c r="AI23" s="61"/>
+      <c r="AJ23" s="61"/>
+      <c r="AK23" s="61"/>
+      <c r="AL23" s="61"/>
       <c r="AM23" s="68"/>
     </row>
     <row r="24" spans="1:39" ht="14.25" customHeight="1">
-      <c r="A24" s="54" t="s">
+      <c r="A24" s="56" t="s">
         <v>39</v>
       </c>
-      <c r="B24" s="82"/>
+      <c r="B24" s="81"/>
       <c r="D24" s="22"/>
       <c r="E24" s="22"/>
       <c r="F24" s="22"/>
@@ -15099,12 +15099,12 @@
       <c r="AD24" s="17"/>
       <c r="AE24" s="6"/>
       <c r="AF24" s="67"/>
-      <c r="AG24" s="63"/>
-      <c r="AH24" s="63"/>
-      <c r="AI24" s="63"/>
-      <c r="AJ24" s="63"/>
-      <c r="AK24" s="63"/>
-      <c r="AL24" s="63"/>
+      <c r="AG24" s="61"/>
+      <c r="AH24" s="61"/>
+      <c r="AI24" s="61"/>
+      <c r="AJ24" s="61"/>
+      <c r="AK24" s="61"/>
+      <c r="AL24" s="61"/>
       <c r="AM24" s="68"/>
     </row>
     <row r="25" spans="1:39" ht="14.25" customHeight="1">
@@ -15142,19 +15142,19 @@
       <c r="AD25" s="17"/>
       <c r="AE25" s="6"/>
       <c r="AF25" s="67"/>
-      <c r="AG25" s="63"/>
-      <c r="AH25" s="63"/>
-      <c r="AI25" s="63"/>
-      <c r="AJ25" s="63"/>
-      <c r="AK25" s="63"/>
-      <c r="AL25" s="63"/>
+      <c r="AG25" s="61"/>
+      <c r="AH25" s="61"/>
+      <c r="AI25" s="61"/>
+      <c r="AJ25" s="61"/>
+      <c r="AK25" s="61"/>
+      <c r="AL25" s="61"/>
       <c r="AM25" s="68"/>
     </row>
     <row r="26" spans="1:39" ht="14.25" customHeight="1">
-      <c r="A26" s="54" t="s">
+      <c r="A26" s="56" t="s">
         <v>40</v>
       </c>
-      <c r="B26" s="82"/>
+      <c r="B26" s="81"/>
       <c r="D26" s="22"/>
       <c r="E26" s="22"/>
       <c r="F26" s="22"/>
@@ -15187,12 +15187,12 @@
       <c r="AD26" s="17"/>
       <c r="AE26" s="6"/>
       <c r="AF26" s="67"/>
-      <c r="AG26" s="63"/>
-      <c r="AH26" s="63"/>
-      <c r="AI26" s="63"/>
-      <c r="AJ26" s="63"/>
-      <c r="AK26" s="63"/>
-      <c r="AL26" s="63"/>
+      <c r="AG26" s="61"/>
+      <c r="AH26" s="61"/>
+      <c r="AI26" s="61"/>
+      <c r="AJ26" s="61"/>
+      <c r="AK26" s="61"/>
+      <c r="AL26" s="61"/>
       <c r="AM26" s="68"/>
     </row>
     <row r="27" spans="1:39" ht="14.25" customHeight="1">
@@ -15230,19 +15230,19 @@
       <c r="AD27" s="17"/>
       <c r="AE27" s="6"/>
       <c r="AF27" s="67"/>
-      <c r="AG27" s="63"/>
-      <c r="AH27" s="63"/>
-      <c r="AI27" s="63"/>
-      <c r="AJ27" s="63"/>
-      <c r="AK27" s="63"/>
-      <c r="AL27" s="63"/>
+      <c r="AG27" s="61"/>
+      <c r="AH27" s="61"/>
+      <c r="AI27" s="61"/>
+      <c r="AJ27" s="61"/>
+      <c r="AK27" s="61"/>
+      <c r="AL27" s="61"/>
       <c r="AM27" s="68"/>
     </row>
     <row r="28" spans="1:39" ht="14.25" customHeight="1">
-      <c r="A28" s="54" t="s">
+      <c r="A28" s="56" t="s">
         <v>41</v>
       </c>
-      <c r="B28" s="82"/>
+      <c r="B28" s="81"/>
       <c r="D28" s="22"/>
       <c r="E28" s="22"/>
       <c r="F28" s="22"/>
@@ -15275,12 +15275,12 @@
       <c r="AD28" s="17"/>
       <c r="AE28" s="6"/>
       <c r="AF28" s="67"/>
-      <c r="AG28" s="63"/>
-      <c r="AH28" s="63"/>
-      <c r="AI28" s="63"/>
-      <c r="AJ28" s="63"/>
-      <c r="AK28" s="63"/>
-      <c r="AL28" s="63"/>
+      <c r="AG28" s="61"/>
+      <c r="AH28" s="61"/>
+      <c r="AI28" s="61"/>
+      <c r="AJ28" s="61"/>
+      <c r="AK28" s="61"/>
+      <c r="AL28" s="61"/>
       <c r="AM28" s="68"/>
     </row>
     <row r="29" spans="1:39" ht="14.25" customHeight="1">
@@ -15318,19 +15318,19 @@
       <c r="AD29" s="17"/>
       <c r="AE29" s="6"/>
       <c r="AF29" s="67"/>
-      <c r="AG29" s="63"/>
-      <c r="AH29" s="63"/>
-      <c r="AI29" s="63"/>
-      <c r="AJ29" s="63"/>
-      <c r="AK29" s="63"/>
-      <c r="AL29" s="63"/>
+      <c r="AG29" s="61"/>
+      <c r="AH29" s="61"/>
+      <c r="AI29" s="61"/>
+      <c r="AJ29" s="61"/>
+      <c r="AK29" s="61"/>
+      <c r="AL29" s="61"/>
       <c r="AM29" s="68"/>
     </row>
     <row r="30" spans="1:39" ht="14.25" customHeight="1">
-      <c r="A30" s="54" t="s">
+      <c r="A30" s="56" t="s">
         <v>42</v>
       </c>
-      <c r="B30" s="83"/>
+      <c r="B30" s="82"/>
       <c r="D30" s="22"/>
       <c r="E30" s="22"/>
       <c r="F30" s="22"/>
@@ -15363,12 +15363,12 @@
       <c r="AD30" s="17"/>
       <c r="AE30" s="6"/>
       <c r="AF30" s="67"/>
-      <c r="AG30" s="63"/>
-      <c r="AH30" s="63"/>
-      <c r="AI30" s="63"/>
-      <c r="AJ30" s="63"/>
-      <c r="AK30" s="63"/>
-      <c r="AL30" s="63"/>
+      <c r="AG30" s="61"/>
+      <c r="AH30" s="61"/>
+      <c r="AI30" s="61"/>
+      <c r="AJ30" s="61"/>
+      <c r="AK30" s="61"/>
+      <c r="AL30" s="61"/>
       <c r="AM30" s="68"/>
     </row>
     <row r="31" spans="1:39" ht="14.25" customHeight="1">
@@ -15406,19 +15406,19 @@
       <c r="AD31" s="17"/>
       <c r="AE31" s="6"/>
       <c r="AF31" s="67"/>
-      <c r="AG31" s="63"/>
-      <c r="AH31" s="63"/>
-      <c r="AI31" s="63"/>
-      <c r="AJ31" s="63"/>
-      <c r="AK31" s="63"/>
-      <c r="AL31" s="63"/>
+      <c r="AG31" s="61"/>
+      <c r="AH31" s="61"/>
+      <c r="AI31" s="61"/>
+      <c r="AJ31" s="61"/>
+      <c r="AK31" s="61"/>
+      <c r="AL31" s="61"/>
       <c r="AM31" s="68"/>
     </row>
     <row r="32" spans="1:39" ht="14.25" customHeight="1">
-      <c r="A32" s="54" t="s">
+      <c r="A32" s="56" t="s">
         <v>43</v>
       </c>
-      <c r="B32" s="83"/>
+      <c r="B32" s="82"/>
       <c r="D32" s="22"/>
       <c r="E32" s="22"/>
       <c r="F32" s="22"/>
@@ -15451,12 +15451,12 @@
       <c r="AD32" s="17"/>
       <c r="AE32" s="6"/>
       <c r="AF32" s="67"/>
-      <c r="AG32" s="63"/>
-      <c r="AH32" s="63"/>
-      <c r="AI32" s="63"/>
-      <c r="AJ32" s="63"/>
-      <c r="AK32" s="63"/>
-      <c r="AL32" s="63"/>
+      <c r="AG32" s="61"/>
+      <c r="AH32" s="61"/>
+      <c r="AI32" s="61"/>
+      <c r="AJ32" s="61"/>
+      <c r="AK32" s="61"/>
+      <c r="AL32" s="61"/>
       <c r="AM32" s="68"/>
     </row>
     <row r="33" spans="1:39" ht="14.25" customHeight="1">
@@ -15494,19 +15494,19 @@
       <c r="AD33" s="17"/>
       <c r="AE33" s="6"/>
       <c r="AF33" s="67"/>
-      <c r="AG33" s="63"/>
-      <c r="AH33" s="63"/>
-      <c r="AI33" s="63"/>
-      <c r="AJ33" s="63"/>
-      <c r="AK33" s="63"/>
-      <c r="AL33" s="63"/>
+      <c r="AG33" s="61"/>
+      <c r="AH33" s="61"/>
+      <c r="AI33" s="61"/>
+      <c r="AJ33" s="61"/>
+      <c r="AK33" s="61"/>
+      <c r="AL33" s="61"/>
       <c r="AM33" s="68"/>
     </row>
     <row r="34" spans="1:39" ht="14.25" customHeight="1">
-      <c r="A34" s="54" t="s">
+      <c r="A34" s="56" t="s">
         <v>44</v>
       </c>
-      <c r="B34" s="83"/>
+      <c r="B34" s="82"/>
       <c r="D34" s="22"/>
       <c r="E34" s="22"/>
       <c r="F34" s="22"/>
@@ -15539,12 +15539,12 @@
       <c r="AD34" s="17"/>
       <c r="AE34" s="6"/>
       <c r="AF34" s="67"/>
-      <c r="AG34" s="63"/>
-      <c r="AH34" s="63"/>
-      <c r="AI34" s="63"/>
-      <c r="AJ34" s="63"/>
-      <c r="AK34" s="63"/>
-      <c r="AL34" s="63"/>
+      <c r="AG34" s="61"/>
+      <c r="AH34" s="61"/>
+      <c r="AI34" s="61"/>
+      <c r="AJ34" s="61"/>
+      <c r="AK34" s="61"/>
+      <c r="AL34" s="61"/>
       <c r="AM34" s="68"/>
     </row>
     <row r="35" spans="1:39" ht="14.25" customHeight="1">
@@ -15582,19 +15582,19 @@
       <c r="AD35" s="17"/>
       <c r="AE35" s="6"/>
       <c r="AF35" s="67"/>
-      <c r="AG35" s="63"/>
-      <c r="AH35" s="63"/>
-      <c r="AI35" s="63"/>
-      <c r="AJ35" s="63"/>
-      <c r="AK35" s="63"/>
-      <c r="AL35" s="63"/>
+      <c r="AG35" s="61"/>
+      <c r="AH35" s="61"/>
+      <c r="AI35" s="61"/>
+      <c r="AJ35" s="61"/>
+      <c r="AK35" s="61"/>
+      <c r="AL35" s="61"/>
       <c r="AM35" s="68"/>
     </row>
     <row r="36" spans="1:39" ht="14.25" customHeight="1">
-      <c r="A36" s="54" t="s">
+      <c r="A36" s="56" t="s">
         <v>123</v>
       </c>
-      <c r="B36" s="83"/>
+      <c r="B36" s="82"/>
       <c r="D36" s="22"/>
       <c r="E36" s="22"/>
       <c r="F36" s="22"/>
@@ -15627,12 +15627,12 @@
       <c r="AD36" s="17"/>
       <c r="AE36" s="6"/>
       <c r="AF36" s="67"/>
-      <c r="AG36" s="63"/>
-      <c r="AH36" s="63"/>
-      <c r="AI36" s="63"/>
-      <c r="AJ36" s="63"/>
-      <c r="AK36" s="63"/>
-      <c r="AL36" s="63"/>
+      <c r="AG36" s="61"/>
+      <c r="AH36" s="61"/>
+      <c r="AI36" s="61"/>
+      <c r="AJ36" s="61"/>
+      <c r="AK36" s="61"/>
+      <c r="AL36" s="61"/>
       <c r="AM36" s="68"/>
     </row>
     <row r="37" spans="1:39" ht="14.25" customHeight="1">
@@ -15679,10 +15679,10 @@
       <c r="AM37" s="71"/>
     </row>
     <row r="38" spans="1:39" ht="14.25" customHeight="1">
-      <c r="A38" s="54" t="s">
+      <c r="A38" s="56" t="s">
         <v>45</v>
       </c>
-      <c r="B38" s="83"/>
+      <c r="B38" s="82"/>
       <c r="D38" s="22"/>
       <c r="E38" s="22"/>
       <c r="F38" s="22"/>
@@ -15767,10 +15767,10 @@
       <c r="AM39" s="52"/>
     </row>
     <row r="40" spans="1:39" ht="17.25" customHeight="1">
-      <c r="A40" s="54" t="s">
+      <c r="A40" s="56" t="s">
         <v>46</v>
       </c>
-      <c r="B40" s="83"/>
+      <c r="B40" s="82"/>
       <c r="D40" s="22"/>
       <c r="E40" s="22"/>
       <c r="F40" s="22"/>
@@ -15855,10 +15855,10 @@
       <c r="AM41" s="52"/>
     </row>
     <row r="42" spans="1:39" ht="17.25" customHeight="1">
-      <c r="A42" s="54" t="s">
+      <c r="A42" s="56" t="s">
         <v>48</v>
       </c>
-      <c r="B42" s="83"/>
+      <c r="B42" s="82"/>
       <c r="D42" s="22"/>
       <c r="E42" s="22"/>
       <c r="F42" s="22"/>
@@ -15943,10 +15943,10 @@
       <c r="AM43" s="52"/>
     </row>
     <row r="44" spans="1:39" ht="17.25" customHeight="1">
-      <c r="A44" s="54" t="s">
+      <c r="A44" s="56" t="s">
         <v>49</v>
       </c>
-      <c r="B44" s="83"/>
+      <c r="B44" s="82"/>
       <c r="D44" s="22"/>
       <c r="E44" s="22"/>
       <c r="F44" s="22"/>
@@ -16022,19 +16022,19 @@
       <c r="AD45" s="17"/>
       <c r="AE45" s="6"/>
       <c r="AF45" s="76"/>
-      <c r="AG45" s="63"/>
-      <c r="AH45" s="63"/>
-      <c r="AI45" s="63"/>
-      <c r="AJ45" s="63"/>
-      <c r="AK45" s="63"/>
-      <c r="AL45" s="63"/>
+      <c r="AG45" s="61"/>
+      <c r="AH45" s="61"/>
+      <c r="AI45" s="61"/>
+      <c r="AJ45" s="61"/>
+      <c r="AK45" s="61"/>
+      <c r="AL45" s="61"/>
       <c r="AM45" s="77"/>
     </row>
     <row r="46" spans="1:39" ht="17.25" customHeight="1">
-      <c r="A46" s="54" t="s">
+      <c r="A46" s="56" t="s">
         <v>50</v>
       </c>
-      <c r="B46" s="83"/>
+      <c r="B46" s="82"/>
       <c r="D46" s="22"/>
       <c r="E46" s="22"/>
       <c r="F46" s="22"/>
@@ -16067,12 +16067,12 @@
       <c r="AD46" s="17"/>
       <c r="AE46" s="6"/>
       <c r="AF46" s="76"/>
-      <c r="AG46" s="63"/>
-      <c r="AH46" s="63"/>
-      <c r="AI46" s="63"/>
-      <c r="AJ46" s="63"/>
-      <c r="AK46" s="63"/>
-      <c r="AL46" s="63"/>
+      <c r="AG46" s="61"/>
+      <c r="AH46" s="61"/>
+      <c r="AI46" s="61"/>
+      <c r="AJ46" s="61"/>
+      <c r="AK46" s="61"/>
+      <c r="AL46" s="61"/>
       <c r="AM46" s="77"/>
     </row>
     <row r="47" spans="1:39" ht="18" customHeight="1">
@@ -16110,19 +16110,19 @@
       <c r="AD47" s="17"/>
       <c r="AE47" s="6"/>
       <c r="AF47" s="76"/>
-      <c r="AG47" s="63"/>
-      <c r="AH47" s="63"/>
-      <c r="AI47" s="63"/>
-      <c r="AJ47" s="63"/>
-      <c r="AK47" s="63"/>
-      <c r="AL47" s="63"/>
+      <c r="AG47" s="61"/>
+      <c r="AH47" s="61"/>
+      <c r="AI47" s="61"/>
+      <c r="AJ47" s="61"/>
+      <c r="AK47" s="61"/>
+      <c r="AL47" s="61"/>
       <c r="AM47" s="77"/>
     </row>
     <row r="48" spans="1:39" ht="14.25" customHeight="1">
-      <c r="A48" s="54" t="s">
+      <c r="A48" s="56" t="s">
         <v>52</v>
       </c>
-      <c r="B48" s="83"/>
+      <c r="B48" s="82"/>
       <c r="D48" s="22"/>
       <c r="E48" s="22"/>
       <c r="F48" s="22"/>
@@ -16155,12 +16155,12 @@
       <c r="AD48" s="17"/>
       <c r="AE48" s="6"/>
       <c r="AF48" s="76"/>
-      <c r="AG48" s="63"/>
-      <c r="AH48" s="63"/>
-      <c r="AI48" s="63"/>
-      <c r="AJ48" s="63"/>
-      <c r="AK48" s="63"/>
-      <c r="AL48" s="63"/>
+      <c r="AG48" s="61"/>
+      <c r="AH48" s="61"/>
+      <c r="AI48" s="61"/>
+      <c r="AJ48" s="61"/>
+      <c r="AK48" s="61"/>
+      <c r="AL48" s="61"/>
       <c r="AM48" s="77"/>
     </row>
     <row r="49" spans="1:39" ht="14.25" customHeight="1">
@@ -16198,19 +16198,19 @@
       <c r="AD49" s="17"/>
       <c r="AE49" s="6"/>
       <c r="AF49" s="76"/>
-      <c r="AG49" s="63"/>
-      <c r="AH49" s="63"/>
-      <c r="AI49" s="63"/>
-      <c r="AJ49" s="63"/>
-      <c r="AK49" s="63"/>
-      <c r="AL49" s="63"/>
+      <c r="AG49" s="61"/>
+      <c r="AH49" s="61"/>
+      <c r="AI49" s="61"/>
+      <c r="AJ49" s="61"/>
+      <c r="AK49" s="61"/>
+      <c r="AL49" s="61"/>
       <c r="AM49" s="77"/>
     </row>
     <row r="50" spans="1:39" ht="17.25" customHeight="1">
-      <c r="A50" s="54" t="s">
+      <c r="A50" s="56" t="s">
         <v>53</v>
       </c>
-      <c r="B50" s="83"/>
+      <c r="B50" s="82"/>
       <c r="D50" s="22"/>
       <c r="E50" s="22"/>
       <c r="F50" s="22"/>
@@ -16243,12 +16243,12 @@
       <c r="AD50" s="17"/>
       <c r="AE50" s="6"/>
       <c r="AF50" s="76"/>
-      <c r="AG50" s="63"/>
-      <c r="AH50" s="63"/>
-      <c r="AI50" s="63"/>
-      <c r="AJ50" s="63"/>
-      <c r="AK50" s="63"/>
-      <c r="AL50" s="63"/>
+      <c r="AG50" s="61"/>
+      <c r="AH50" s="61"/>
+      <c r="AI50" s="61"/>
+      <c r="AJ50" s="61"/>
+      <c r="AK50" s="61"/>
+      <c r="AL50" s="61"/>
       <c r="AM50" s="77"/>
     </row>
     <row r="51" spans="1:39" ht="18" customHeight="1">
@@ -16286,19 +16286,19 @@
       <c r="AD51" s="17"/>
       <c r="AE51" s="6"/>
       <c r="AF51" s="76"/>
-      <c r="AG51" s="63"/>
-      <c r="AH51" s="63"/>
-      <c r="AI51" s="63"/>
-      <c r="AJ51" s="63"/>
-      <c r="AK51" s="63"/>
-      <c r="AL51" s="63"/>
+      <c r="AG51" s="61"/>
+      <c r="AH51" s="61"/>
+      <c r="AI51" s="61"/>
+      <c r="AJ51" s="61"/>
+      <c r="AK51" s="61"/>
+      <c r="AL51" s="61"/>
       <c r="AM51" s="77"/>
     </row>
     <row r="52" spans="1:39" ht="17.25" customHeight="1">
-      <c r="A52" s="54" t="s">
+      <c r="A52" s="56" t="s">
         <v>54</v>
       </c>
-      <c r="B52" s="83"/>
+      <c r="B52" s="82"/>
       <c r="D52" s="22"/>
       <c r="E52" s="22"/>
       <c r="F52" s="22"/>
@@ -16331,12 +16331,12 @@
       <c r="AD52" s="17"/>
       <c r="AE52" s="6"/>
       <c r="AF52" s="76"/>
-      <c r="AG52" s="63"/>
-      <c r="AH52" s="63"/>
-      <c r="AI52" s="63"/>
-      <c r="AJ52" s="63"/>
-      <c r="AK52" s="63"/>
-      <c r="AL52" s="63"/>
+      <c r="AG52" s="61"/>
+      <c r="AH52" s="61"/>
+      <c r="AI52" s="61"/>
+      <c r="AJ52" s="61"/>
+      <c r="AK52" s="61"/>
+      <c r="AL52" s="61"/>
       <c r="AM52" s="77"/>
     </row>
     <row r="53" spans="1:39" ht="18" customHeight="1">
@@ -16374,19 +16374,19 @@
       <c r="AD53" s="17"/>
       <c r="AE53" s="6"/>
       <c r="AF53" s="76"/>
-      <c r="AG53" s="63"/>
-      <c r="AH53" s="63"/>
-      <c r="AI53" s="63"/>
-      <c r="AJ53" s="63"/>
-      <c r="AK53" s="63"/>
-      <c r="AL53" s="63"/>
+      <c r="AG53" s="61"/>
+      <c r="AH53" s="61"/>
+      <c r="AI53" s="61"/>
+      <c r="AJ53" s="61"/>
+      <c r="AK53" s="61"/>
+      <c r="AL53" s="61"/>
       <c r="AM53" s="77"/>
     </row>
     <row r="54" spans="1:39" ht="17.25" customHeight="1">
-      <c r="A54" s="54" t="s">
+      <c r="A54" s="56" t="s">
         <v>55</v>
       </c>
-      <c r="B54" s="83"/>
+      <c r="B54" s="82"/>
       <c r="D54" s="22"/>
       <c r="E54" s="22"/>
       <c r="F54" s="22"/>
@@ -16419,12 +16419,12 @@
       <c r="AD54" s="17"/>
       <c r="AE54" s="6"/>
       <c r="AF54" s="76"/>
-      <c r="AG54" s="63"/>
-      <c r="AH54" s="63"/>
-      <c r="AI54" s="63"/>
-      <c r="AJ54" s="63"/>
-      <c r="AK54" s="63"/>
-      <c r="AL54" s="63"/>
+      <c r="AG54" s="61"/>
+      <c r="AH54" s="61"/>
+      <c r="AI54" s="61"/>
+      <c r="AJ54" s="61"/>
+      <c r="AK54" s="61"/>
+      <c r="AL54" s="61"/>
       <c r="AM54" s="77"/>
     </row>
     <row r="55" spans="1:39" ht="18" customHeight="1">
@@ -16462,19 +16462,19 @@
       <c r="AD55" s="17"/>
       <c r="AE55" s="6"/>
       <c r="AF55" s="76"/>
-      <c r="AG55" s="63"/>
-      <c r="AH55" s="63"/>
-      <c r="AI55" s="63"/>
-      <c r="AJ55" s="63"/>
-      <c r="AK55" s="63"/>
-      <c r="AL55" s="63"/>
+      <c r="AG55" s="61"/>
+      <c r="AH55" s="61"/>
+      <c r="AI55" s="61"/>
+      <c r="AJ55" s="61"/>
+      <c r="AK55" s="61"/>
+      <c r="AL55" s="61"/>
       <c r="AM55" s="77"/>
     </row>
     <row r="56" spans="1:39" ht="14.25" customHeight="1">
-      <c r="A56" s="54" t="s">
+      <c r="A56" s="56" t="s">
         <v>78</v>
       </c>
-      <c r="B56" s="83"/>
+      <c r="B56" s="82"/>
       <c r="D56" s="22"/>
       <c r="E56" s="22"/>
       <c r="F56" s="22"/>
@@ -16507,12 +16507,12 @@
       <c r="AD56" s="17"/>
       <c r="AE56" s="6"/>
       <c r="AF56" s="76"/>
-      <c r="AG56" s="63"/>
-      <c r="AH56" s="63"/>
-      <c r="AI56" s="63"/>
-      <c r="AJ56" s="63"/>
-      <c r="AK56" s="63"/>
-      <c r="AL56" s="63"/>
+      <c r="AG56" s="61"/>
+      <c r="AH56" s="61"/>
+      <c r="AI56" s="61"/>
+      <c r="AJ56" s="61"/>
+      <c r="AK56" s="61"/>
+      <c r="AL56" s="61"/>
       <c r="AM56" s="77"/>
     </row>
     <row r="57" spans="1:39" ht="14.25" customHeight="1">
@@ -16550,19 +16550,19 @@
       <c r="AD57" s="17"/>
       <c r="AE57" s="6"/>
       <c r="AF57" s="76"/>
-      <c r="AG57" s="63"/>
-      <c r="AH57" s="63"/>
-      <c r="AI57" s="63"/>
-      <c r="AJ57" s="63"/>
-      <c r="AK57" s="63"/>
-      <c r="AL57" s="63"/>
+      <c r="AG57" s="61"/>
+      <c r="AH57" s="61"/>
+      <c r="AI57" s="61"/>
+      <c r="AJ57" s="61"/>
+      <c r="AK57" s="61"/>
+      <c r="AL57" s="61"/>
       <c r="AM57" s="77"/>
     </row>
     <row r="58" spans="1:39" ht="17.25" customHeight="1">
-      <c r="A58" s="54" t="s">
+      <c r="A58" s="56" t="s">
         <v>79</v>
       </c>
-      <c r="B58" s="83"/>
+      <c r="B58" s="82"/>
       <c r="D58" s="22"/>
       <c r="E58" s="22"/>
       <c r="F58" s="22"/>
@@ -16595,12 +16595,12 @@
       <c r="AD58" s="17"/>
       <c r="AE58" s="6"/>
       <c r="AF58" s="76"/>
-      <c r="AG58" s="63"/>
-      <c r="AH58" s="63"/>
-      <c r="AI58" s="63"/>
-      <c r="AJ58" s="63"/>
-      <c r="AK58" s="63"/>
-      <c r="AL58" s="63"/>
+      <c r="AG58" s="61"/>
+      <c r="AH58" s="61"/>
+      <c r="AI58" s="61"/>
+      <c r="AJ58" s="61"/>
+      <c r="AK58" s="61"/>
+      <c r="AL58" s="61"/>
       <c r="AM58" s="77"/>
     </row>
     <row r="59" spans="1:39" ht="18" customHeight="1">
@@ -16638,19 +16638,19 @@
       <c r="AD59" s="17"/>
       <c r="AE59" s="6"/>
       <c r="AF59" s="76"/>
-      <c r="AG59" s="63"/>
-      <c r="AH59" s="63"/>
-      <c r="AI59" s="63"/>
-      <c r="AJ59" s="63"/>
-      <c r="AK59" s="63"/>
-      <c r="AL59" s="63"/>
+      <c r="AG59" s="61"/>
+      <c r="AH59" s="61"/>
+      <c r="AI59" s="61"/>
+      <c r="AJ59" s="61"/>
+      <c r="AK59" s="61"/>
+      <c r="AL59" s="61"/>
       <c r="AM59" s="77"/>
     </row>
     <row r="60" spans="1:39" ht="17.25" customHeight="1">
-      <c r="A60" s="54" t="s">
+      <c r="A60" s="56" t="s">
         <v>81</v>
       </c>
-      <c r="B60" s="83"/>
+      <c r="B60" s="82"/>
       <c r="D60" s="22"/>
       <c r="E60" s="22"/>
       <c r="F60" s="22"/>
@@ -16683,12 +16683,12 @@
       <c r="AD60" s="17"/>
       <c r="AE60" s="6"/>
       <c r="AF60" s="76"/>
-      <c r="AG60" s="63"/>
-      <c r="AH60" s="63"/>
-      <c r="AI60" s="63"/>
-      <c r="AJ60" s="63"/>
-      <c r="AK60" s="63"/>
-      <c r="AL60" s="63"/>
+      <c r="AG60" s="61"/>
+      <c r="AH60" s="61"/>
+      <c r="AI60" s="61"/>
+      <c r="AJ60" s="61"/>
+      <c r="AK60" s="61"/>
+      <c r="AL60" s="61"/>
       <c r="AM60" s="77"/>
     </row>
     <row r="61" spans="1:39" ht="18" customHeight="1">
@@ -16726,19 +16726,19 @@
       <c r="AD61" s="17"/>
       <c r="AE61" s="6"/>
       <c r="AF61" s="76"/>
-      <c r="AG61" s="63"/>
-      <c r="AH61" s="63"/>
-      <c r="AI61" s="63"/>
-      <c r="AJ61" s="63"/>
-      <c r="AK61" s="63"/>
-      <c r="AL61" s="63"/>
+      <c r="AG61" s="61"/>
+      <c r="AH61" s="61"/>
+      <c r="AI61" s="61"/>
+      <c r="AJ61" s="61"/>
+      <c r="AK61" s="61"/>
+      <c r="AL61" s="61"/>
       <c r="AM61" s="77"/>
     </row>
     <row r="62" spans="1:39" ht="17.25" customHeight="1">
-      <c r="A62" s="54" t="s">
+      <c r="A62" s="56" t="s">
         <v>82</v>
       </c>
-      <c r="B62" s="83"/>
+      <c r="B62" s="82"/>
       <c r="D62" s="22"/>
       <c r="E62" s="22"/>
       <c r="F62" s="22"/>
@@ -16771,12 +16771,12 @@
       <c r="AD62" s="17"/>
       <c r="AE62" s="6"/>
       <c r="AF62" s="76"/>
-      <c r="AG62" s="63"/>
-      <c r="AH62" s="63"/>
-      <c r="AI62" s="63"/>
-      <c r="AJ62" s="63"/>
-      <c r="AK62" s="63"/>
-      <c r="AL62" s="63"/>
+      <c r="AG62" s="61"/>
+      <c r="AH62" s="61"/>
+      <c r="AI62" s="61"/>
+      <c r="AJ62" s="61"/>
+      <c r="AK62" s="61"/>
+      <c r="AL62" s="61"/>
       <c r="AM62" s="77"/>
     </row>
     <row r="63" spans="1:39" ht="18" customHeight="1">
@@ -16814,19 +16814,19 @@
       <c r="AD63" s="32"/>
       <c r="AE63" s="6"/>
       <c r="AF63" s="76"/>
-      <c r="AG63" s="63"/>
-      <c r="AH63" s="63"/>
-      <c r="AI63" s="63"/>
-      <c r="AJ63" s="63"/>
-      <c r="AK63" s="63"/>
-      <c r="AL63" s="63"/>
+      <c r="AG63" s="61"/>
+      <c r="AH63" s="61"/>
+      <c r="AI63" s="61"/>
+      <c r="AJ63" s="61"/>
+      <c r="AK63" s="61"/>
+      <c r="AL63" s="61"/>
       <c r="AM63" s="77"/>
     </row>
     <row r="64" spans="1:39" ht="17.25" customHeight="1">
-      <c r="A64" s="54" t="s">
+      <c r="A64" s="56" t="s">
         <v>84</v>
       </c>
-      <c r="B64" s="83"/>
+      <c r="B64" s="82"/>
       <c r="D64" s="22"/>
       <c r="E64" s="22"/>
       <c r="F64" s="22"/>
@@ -16859,12 +16859,12 @@
       <c r="AD64" s="32"/>
       <c r="AE64" s="6"/>
       <c r="AF64" s="76"/>
-      <c r="AG64" s="63"/>
-      <c r="AH64" s="63"/>
-      <c r="AI64" s="63"/>
-      <c r="AJ64" s="63"/>
-      <c r="AK64" s="63"/>
-      <c r="AL64" s="63"/>
+      <c r="AG64" s="61"/>
+      <c r="AH64" s="61"/>
+      <c r="AI64" s="61"/>
+      <c r="AJ64" s="61"/>
+      <c r="AK64" s="61"/>
+      <c r="AL64" s="61"/>
       <c r="AM64" s="77"/>
     </row>
     <row r="65" spans="1:39" ht="18" customHeight="1">
@@ -16902,19 +16902,19 @@
       <c r="AD65" s="32"/>
       <c r="AE65" s="6"/>
       <c r="AF65" s="76"/>
-      <c r="AG65" s="63"/>
-      <c r="AH65" s="63"/>
-      <c r="AI65" s="63"/>
-      <c r="AJ65" s="63"/>
-      <c r="AK65" s="63"/>
-      <c r="AL65" s="63"/>
+      <c r="AG65" s="61"/>
+      <c r="AH65" s="61"/>
+      <c r="AI65" s="61"/>
+      <c r="AJ65" s="61"/>
+      <c r="AK65" s="61"/>
+      <c r="AL65" s="61"/>
       <c r="AM65" s="77"/>
     </row>
     <row r="66" spans="1:39" ht="14.25" customHeight="1">
-      <c r="A66" s="54" t="s">
+      <c r="A66" s="56" t="s">
         <v>52</v>
       </c>
-      <c r="B66" s="57"/>
+      <c r="B66" s="54"/>
       <c r="D66" s="22"/>
       <c r="E66" s="22"/>
       <c r="F66" s="22"/>
@@ -16947,12 +16947,12 @@
       <c r="AD66" s="17"/>
       <c r="AE66" s="6"/>
       <c r="AF66" s="76"/>
-      <c r="AG66" s="63"/>
-      <c r="AH66" s="63"/>
-      <c r="AI66" s="63"/>
-      <c r="AJ66" s="63"/>
-      <c r="AK66" s="63"/>
-      <c r="AL66" s="63"/>
+      <c r="AG66" s="61"/>
+      <c r="AH66" s="61"/>
+      <c r="AI66" s="61"/>
+      <c r="AJ66" s="61"/>
+      <c r="AK66" s="61"/>
+      <c r="AL66" s="61"/>
       <c r="AM66" s="77"/>
     </row>
     <row r="67" spans="1:39" ht="14.25" customHeight="1">
@@ -16990,19 +16990,19 @@
       <c r="AD67" s="17"/>
       <c r="AE67" s="6"/>
       <c r="AF67" s="76"/>
-      <c r="AG67" s="63"/>
-      <c r="AH67" s="63"/>
-      <c r="AI67" s="63"/>
-      <c r="AJ67" s="63"/>
-      <c r="AK67" s="63"/>
-      <c r="AL67" s="63"/>
+      <c r="AG67" s="61"/>
+      <c r="AH67" s="61"/>
+      <c r="AI67" s="61"/>
+      <c r="AJ67" s="61"/>
+      <c r="AK67" s="61"/>
+      <c r="AL67" s="61"/>
       <c r="AM67" s="77"/>
     </row>
     <row r="68" spans="1:39" ht="14.25" customHeight="1">
-      <c r="A68" s="54" t="s">
+      <c r="A68" s="56" t="s">
         <v>53</v>
       </c>
-      <c r="B68" s="57"/>
+      <c r="B68" s="54"/>
       <c r="D68" s="22"/>
       <c r="E68" s="22"/>
       <c r="F68" s="22"/>
@@ -17035,12 +17035,12 @@
       <c r="AD68" s="17"/>
       <c r="AE68" s="6"/>
       <c r="AF68" s="76"/>
-      <c r="AG68" s="63"/>
-      <c r="AH68" s="63"/>
-      <c r="AI68" s="63"/>
-      <c r="AJ68" s="63"/>
-      <c r="AK68" s="63"/>
-      <c r="AL68" s="63"/>
+      <c r="AG68" s="61"/>
+      <c r="AH68" s="61"/>
+      <c r="AI68" s="61"/>
+      <c r="AJ68" s="61"/>
+      <c r="AK68" s="61"/>
+      <c r="AL68" s="61"/>
       <c r="AM68" s="77"/>
     </row>
     <row r="69" spans="1:39" ht="14.25" customHeight="1">
@@ -17078,19 +17078,19 @@
       <c r="AD69" s="17"/>
       <c r="AE69" s="6"/>
       <c r="AF69" s="76"/>
-      <c r="AG69" s="63"/>
-      <c r="AH69" s="63"/>
-      <c r="AI69" s="63"/>
-      <c r="AJ69" s="63"/>
-      <c r="AK69" s="63"/>
-      <c r="AL69" s="63"/>
+      <c r="AG69" s="61"/>
+      <c r="AH69" s="61"/>
+      <c r="AI69" s="61"/>
+      <c r="AJ69" s="61"/>
+      <c r="AK69" s="61"/>
+      <c r="AL69" s="61"/>
       <c r="AM69" s="77"/>
     </row>
     <row r="70" spans="1:39" ht="14.25" customHeight="1">
-      <c r="A70" s="54" t="s">
+      <c r="A70" s="56" t="s">
         <v>54</v>
       </c>
-      <c r="B70" s="57"/>
+      <c r="B70" s="54"/>
       <c r="D70" s="22"/>
       <c r="E70" s="22"/>
       <c r="F70" s="22"/>
@@ -17123,12 +17123,12 @@
       <c r="AD70" s="17"/>
       <c r="AE70" s="6"/>
       <c r="AF70" s="76"/>
-      <c r="AG70" s="63"/>
-      <c r="AH70" s="63"/>
-      <c r="AI70" s="63"/>
-      <c r="AJ70" s="63"/>
-      <c r="AK70" s="63"/>
-      <c r="AL70" s="63"/>
+      <c r="AG70" s="61"/>
+      <c r="AH70" s="61"/>
+      <c r="AI70" s="61"/>
+      <c r="AJ70" s="61"/>
+      <c r="AK70" s="61"/>
+      <c r="AL70" s="61"/>
       <c r="AM70" s="77"/>
     </row>
     <row r="71" spans="1:39" ht="14.25" customHeight="1">
@@ -17166,19 +17166,19 @@
       <c r="AD71" s="17"/>
       <c r="AE71" s="6"/>
       <c r="AF71" s="76"/>
-      <c r="AG71" s="63"/>
-      <c r="AH71" s="63"/>
-      <c r="AI71" s="63"/>
-      <c r="AJ71" s="63"/>
-      <c r="AK71" s="63"/>
-      <c r="AL71" s="63"/>
+      <c r="AG71" s="61"/>
+      <c r="AH71" s="61"/>
+      <c r="AI71" s="61"/>
+      <c r="AJ71" s="61"/>
+      <c r="AK71" s="61"/>
+      <c r="AL71" s="61"/>
       <c r="AM71" s="77"/>
     </row>
     <row r="72" spans="1:39" ht="14.25" customHeight="1">
-      <c r="A72" s="54" t="s">
+      <c r="A72" s="56" t="s">
         <v>55</v>
       </c>
-      <c r="B72" s="57"/>
+      <c r="B72" s="54"/>
       <c r="D72" s="22"/>
       <c r="E72" s="22"/>
       <c r="F72" s="22"/>
@@ -17265,10 +17265,10 @@
       <c r="AM73" s="38"/>
     </row>
     <row r="74" spans="1:39" ht="14.25" customHeight="1">
-      <c r="A74" s="54" t="s">
+      <c r="A74" s="56" t="s">
         <v>56</v>
       </c>
-      <c r="B74" s="57"/>
+      <c r="B74" s="54"/>
       <c r="D74" s="22"/>
       <c r="E74" s="22"/>
       <c r="F74" s="22"/>
@@ -17357,8 +17357,8 @@
       <c r="AM75" s="38"/>
     </row>
     <row r="76" spans="1:39" ht="14.25" customHeight="1">
-      <c r="A76" s="81"/>
-      <c r="B76" s="81"/>
+      <c r="A76" s="83"/>
+      <c r="B76" s="83"/>
       <c r="D76" s="22"/>
       <c r="E76" s="22"/>
       <c r="F76" s="22"/>
@@ -17447,8 +17447,8 @@
       <c r="AM77" s="38"/>
     </row>
     <row r="78" spans="1:39" ht="14.25" customHeight="1">
-      <c r="A78" s="81"/>
-      <c r="B78" s="81"/>
+      <c r="A78" s="83"/>
+      <c r="B78" s="83"/>
       <c r="D78" s="22"/>
       <c r="E78" s="22"/>
       <c r="F78" s="22"/>
@@ -17535,8 +17535,8 @@
       <c r="AM79" s="38"/>
     </row>
     <row r="80" spans="1:39" ht="14.25" customHeight="1">
-      <c r="A80" s="81"/>
-      <c r="B80" s="81"/>
+      <c r="A80" s="83"/>
+      <c r="B80" s="83"/>
       <c r="D80" s="22"/>
       <c r="E80" s="22"/>
       <c r="F80" s="22"/>
@@ -18580,9 +18580,6 @@
     <row r="1000" ht="14.25" customHeight="1"/>
   </sheetData>
   <mergeCells count="81">
-    <mergeCell ref="A64:A65"/>
-    <mergeCell ref="A66:A67"/>
-    <mergeCell ref="A68:A69"/>
     <mergeCell ref="A70:A71"/>
     <mergeCell ref="B80:B81"/>
     <mergeCell ref="A72:A73"/>
@@ -18590,32 +18587,22 @@
     <mergeCell ref="A76:A77"/>
     <mergeCell ref="A78:A79"/>
     <mergeCell ref="A80:A81"/>
-    <mergeCell ref="B64:B65"/>
     <mergeCell ref="B72:B73"/>
     <mergeCell ref="B74:B75"/>
     <mergeCell ref="B76:B77"/>
     <mergeCell ref="B78:B79"/>
-    <mergeCell ref="A54:A55"/>
-    <mergeCell ref="A56:A57"/>
-    <mergeCell ref="B58:B59"/>
-    <mergeCell ref="B60:B61"/>
-    <mergeCell ref="B62:B63"/>
-    <mergeCell ref="A58:A59"/>
-    <mergeCell ref="A60:A61"/>
-    <mergeCell ref="A62:A63"/>
     <mergeCell ref="A6:A7"/>
     <mergeCell ref="A46:A47"/>
     <mergeCell ref="A48:A49"/>
     <mergeCell ref="A50:A51"/>
     <mergeCell ref="A52:A53"/>
-    <mergeCell ref="B66:B67"/>
-    <mergeCell ref="B68:B69"/>
-    <mergeCell ref="AA1:AD1"/>
-    <mergeCell ref="D3:G3"/>
-    <mergeCell ref="AF3:AM37"/>
-    <mergeCell ref="D4:G4"/>
-    <mergeCell ref="B6:B7"/>
-    <mergeCell ref="B8:B9"/>
+    <mergeCell ref="A32:A33"/>
+    <mergeCell ref="A34:A35"/>
+    <mergeCell ref="A24:A25"/>
+    <mergeCell ref="A18:A19"/>
+    <mergeCell ref="A8:A9"/>
+    <mergeCell ref="A10:A11"/>
+    <mergeCell ref="A14:A15"/>
     <mergeCell ref="AF44:AM72"/>
     <mergeCell ref="B70:B71"/>
     <mergeCell ref="B46:B47"/>
@@ -18624,37 +18611,50 @@
     <mergeCell ref="B52:B53"/>
     <mergeCell ref="B54:B55"/>
     <mergeCell ref="B56:B57"/>
-    <mergeCell ref="A32:A33"/>
+    <mergeCell ref="B58:B59"/>
+    <mergeCell ref="B60:B61"/>
+    <mergeCell ref="B62:B63"/>
+    <mergeCell ref="B64:B65"/>
+    <mergeCell ref="B66:B67"/>
+    <mergeCell ref="AA1:AD1"/>
+    <mergeCell ref="D3:G3"/>
+    <mergeCell ref="AF3:AM37"/>
+    <mergeCell ref="D4:G4"/>
+    <mergeCell ref="B6:B7"/>
+    <mergeCell ref="B8:B9"/>
     <mergeCell ref="B32:B33"/>
-    <mergeCell ref="A34:A35"/>
-    <mergeCell ref="B34:B35"/>
-    <mergeCell ref="A36:A37"/>
-    <mergeCell ref="B36:B37"/>
     <mergeCell ref="A42:A43"/>
     <mergeCell ref="A44:A45"/>
-    <mergeCell ref="A24:A25"/>
+    <mergeCell ref="B42:B43"/>
+    <mergeCell ref="B44:B45"/>
+    <mergeCell ref="B68:B69"/>
+    <mergeCell ref="A54:A55"/>
+    <mergeCell ref="A56:A57"/>
+    <mergeCell ref="A58:A59"/>
+    <mergeCell ref="A60:A61"/>
+    <mergeCell ref="A62:A63"/>
+    <mergeCell ref="A64:A65"/>
+    <mergeCell ref="A66:A67"/>
+    <mergeCell ref="A68:A69"/>
     <mergeCell ref="B24:B25"/>
     <mergeCell ref="A38:A39"/>
     <mergeCell ref="B38:B39"/>
     <mergeCell ref="A40:A41"/>
     <mergeCell ref="B40:B41"/>
-    <mergeCell ref="B42:B43"/>
-    <mergeCell ref="B44:B45"/>
     <mergeCell ref="A26:A27"/>
     <mergeCell ref="B26:B27"/>
     <mergeCell ref="A28:A29"/>
     <mergeCell ref="B28:B29"/>
     <mergeCell ref="A30:A31"/>
     <mergeCell ref="B30:B31"/>
-    <mergeCell ref="A18:A19"/>
+    <mergeCell ref="B34:B35"/>
+    <mergeCell ref="A36:A37"/>
+    <mergeCell ref="B36:B37"/>
     <mergeCell ref="B18:B19"/>
     <mergeCell ref="A20:A21"/>
     <mergeCell ref="B20:B21"/>
     <mergeCell ref="A22:A23"/>
     <mergeCell ref="B22:B23"/>
-    <mergeCell ref="A8:A9"/>
-    <mergeCell ref="A10:A11"/>
-    <mergeCell ref="A14:A15"/>
     <mergeCell ref="B14:B15"/>
     <mergeCell ref="A16:A17"/>
     <mergeCell ref="B16:B17"/>

</xml_diff>